<commit_message>
Implemented SREPL. Added parallel processing to POS,POSREVand NPOS,NPOSREV for strings.
</commit_message>
<xml_diff>
--- a/newrpl/docs/newRPLCommandDatabase.xlsx
+++ b/newrpl/docs/newRPLCommandDatabase.xlsx
@@ -28,9 +28,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="985">
   <si>
     <t xml:space="preserve">Total commands implemented</t>
   </si>
@@ -3014,6 +3015,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3036,24 +3038,28 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -3061,24 +3067,28 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3086,6 +3096,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3093,12 +3104,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3106,12 +3119,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3119,6 +3134,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3126,6 +3142,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3133,6 +3150,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="17">
@@ -3515,9 +3533,9 @@
   <dimension ref="A2:J1121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="5" topLeftCell="A738" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1002" activeCellId="0" sqref="C1002"/>
+      <selection pane="bottomLeft" activeCell="C841" activeCellId="0" sqref="C841"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3540,7 +3558,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="n">
         <f aca="false">COUNTIF(J6:J1001,1)</f>
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>1</v>
@@ -3556,7 +3574,7 @@
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">D2/F2</f>
-        <v>0.43</v>
+        <v>0.43125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6537,7 +6555,7 @@
       <c r="B134" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -13572,7 +13590,7 @@
       <c r="B443" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="C443" s="1" t="s">
+      <c r="C443" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D443" s="1" t="s">
@@ -18111,9 +18129,13 @@
       <c r="B640" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="C640" s="1" t="s">
+      <c r="C640" s="12" t="s">
         <v>170</v>
       </c>
+      <c r="D640" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F640" s="16"/>
       <c r="G640" s="1"/>
       <c r="H640" s="0" t="n">
         <v>120</v>
@@ -18124,7 +18146,7 @@
       </c>
       <c r="J640" s="0" t="n">
         <f aca="false">IF(ISBLANK(D640),0,I640)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23590,7 +23612,7 @@
       <c r="B877" s="2" t="s">
         <v>955</v>
       </c>
-      <c r="C877" s="1" t="s">
+      <c r="C877" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D877" s="1" t="s">
@@ -23614,7 +23636,7 @@
       <c r="B878" s="2" t="s">
         <v>956</v>
       </c>
-      <c r="C878" s="1" t="s">
+      <c r="C878" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D878" s="1" t="s">
@@ -23638,7 +23660,7 @@
       <c r="B879" s="2" t="s">
         <v>957</v>
       </c>
-      <c r="C879" s="1" t="s">
+      <c r="C879" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D879" s="1" t="s">
@@ -23662,7 +23684,7 @@
       <c r="B880" s="2" t="s">
         <v>958</v>
       </c>
-      <c r="C880" s="1" t="s">
+      <c r="C880" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D880" s="1" t="s">
@@ -23686,7 +23708,7 @@
       <c r="B881" s="2" t="s">
         <v>959</v>
       </c>
-      <c r="C881" s="1" t="s">
+      <c r="C881" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D881" s="1" t="s">
@@ -23710,7 +23732,7 @@
       <c r="B882" s="2" t="s">
         <v>960</v>
       </c>
-      <c r="C882" s="1" t="s">
+      <c r="C882" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D882" s="1" t="s">
@@ -23734,7 +23756,7 @@
       <c r="B883" s="2" t="s">
         <v>961</v>
       </c>
-      <c r="C883" s="1" t="s">
+      <c r="C883" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D883" s="1" t="s">
@@ -23758,7 +23780,7 @@
       <c r="B884" s="2" t="s">
         <v>962</v>
       </c>
-      <c r="C884" s="1" t="s">
+      <c r="C884" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D884" s="1" t="s">
@@ -23782,7 +23804,7 @@
       <c r="B885" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="C885" s="1" t="s">
+      <c r="C885" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D885" s="1" t="s">
@@ -23806,7 +23828,7 @@
       <c r="B886" s="2" t="s">
         <v>964</v>
       </c>
-      <c r="C886" s="1" t="s">
+      <c r="C886" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D886" s="1" t="s">
@@ -24046,7 +24068,7 @@
       <c r="B896" s="2" t="s">
         <v>974</v>
       </c>
-      <c r="C896" s="1" t="s">
+      <c r="C896" s="12" t="s">
         <v>170</v>
       </c>
       <c r="D896" s="1" t="s">

</xml_diff>

<commit_message>
Added polynomial solver. Implemented PROOT.
</commit_message>
<xml_diff>
--- a/newrpl/docs/newRPLCommandDatabase.xlsx
+++ b/newrpl/docs/newRPLCommandDatabase.xlsx
@@ -42,9 +42,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2466" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="1022">
   <si>
     <t xml:space="preserve">Total commands implemented</t>
   </si>
@@ -3477,9 +3479,9 @@
   <dimension ref="A2:J1121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="5" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D343" activeCellId="0" sqref="D343"/>
+      <selection pane="bottomLeft" activeCell="D233" activeCellId="0" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3502,7 +3504,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="n">
         <f aca="false">COUNTIF(J6:J1001,1)</f>
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>1</v>
@@ -3518,7 +3520,7 @@
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">D2/F2</f>
-        <v>0.51063829787234</v>
+        <v>0.514392991239049</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8443,6 +8445,9 @@
       <c r="C215" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D215" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G215" s="1"/>
       <c r="H215" s="0" t="n">
         <v>110</v>
@@ -8453,7 +8458,7 @@
       </c>
       <c r="J215" s="0" t="n">
         <f aca="false">IF(ISBLANK(D215),0,I215)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11391,6 +11396,9 @@
       <c r="C343" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D343" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G343" s="1"/>
       <c r="H343" s="0" t="n">
         <v>110</v>
@@ -11401,7 +11409,7 @@
       </c>
       <c r="J343" s="0" t="n">
         <f aca="false">IF(ISBLANK(D343),0,I343)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11784,6 +11792,9 @@
       <c r="C360" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D360" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G360" s="1"/>
       <c r="H360" s="0" t="n">
         <v>110</v>
@@ -11794,7 +11805,7 @@
       </c>
       <c r="J360" s="0" t="n">
         <f aca="false">IF(ISBLANK(D360),0,I360)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added several matrix commands.
</commit_message>
<xml_diff>
--- a/newrpl/docs/newRPLCommandDatabase.xlsx
+++ b/newrpl/docs/newRPLCommandDatabase.xlsx
@@ -49,9 +49,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2486" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="1026">
   <si>
     <t xml:space="preserve">Total commands implemented</t>
   </si>
@@ -1939,6 +1940,9 @@
     <t xml:space="preserve">REF</t>
   </si>
   <si>
+    <t xml:space="preserve">Uses Bareiss algorithm</t>
+  </si>
+  <si>
     <t xml:space="preserve">REMAINDER</t>
   </si>
   <si>
@@ -2039,6 +2043,9 @@
   </si>
   <si>
     <t xml:space="preserve">RREF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step-by-step mode not supported</t>
   </si>
   <si>
     <t xml:space="preserve">RREFMOD</t>
@@ -3500,9 +3507,9 @@
   <dimension ref="A2:J1121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="5" topLeftCell="A422" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="D599" activeCellId="0" sqref="D599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3525,7 +3532,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="n">
         <f aca="false">COUNTIF(J6:J1001,1)</f>
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>1</v>
@@ -3541,7 +3548,7 @@
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">D2/F2</f>
-        <v>0.525188916876574</v>
+        <v>0.535264483627204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15903,6 +15910,9 @@
       <c r="C536" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D536" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G536" s="1"/>
       <c r="H536" s="0" t="n">
         <v>110</v>
@@ -15913,7 +15923,7 @@
       </c>
       <c r="J536" s="0" t="n">
         <f aca="false">IF(ISBLANK(D536),0,I536)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15969,6 +15979,9 @@
       <c r="C539" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D539" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G539" s="1"/>
       <c r="H539" s="0" t="n">
         <v>110</v>
@@ -15979,7 +15992,7 @@
       </c>
       <c r="J539" s="0" t="n">
         <f aca="false">IF(ISBLANK(D539),0,I539)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15993,6 +16006,9 @@
       <c r="C540" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D540" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G540" s="1"/>
       <c r="H540" s="0" t="n">
         <v>110</v>
@@ -16003,7 +16019,7 @@
       </c>
       <c r="J540" s="0" t="n">
         <f aca="false">IF(ISBLANK(D540),0,I540)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16210,6 +16226,9 @@
       <c r="C549" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D549" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G549" s="1"/>
       <c r="H549" s="0" t="n">
         <v>110</v>
@@ -16220,7 +16239,7 @@
       </c>
       <c r="J549" s="0" t="n">
         <f aca="false">IF(ISBLANK(D549),0,I549)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16357,7 +16376,13 @@
       <c r="C555" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G555" s="1"/>
+      <c r="D555" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E555" s="22"/>
+      <c r="G555" s="1" t="s">
+        <v>624</v>
+      </c>
       <c r="H555" s="0" t="n">
         <v>110</v>
       </c>
@@ -16367,7 +16392,7 @@
       </c>
       <c r="J555" s="0" t="n">
         <f aca="false">IF(ISBLANK(D555),0,I555)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16376,7 +16401,7 @@
         <v>550</v>
       </c>
       <c r="B556" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C556" s="1" t="s">
         <v>27</v>
@@ -16397,7 +16422,7 @@
         <v>551</v>
       </c>
       <c r="B557" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C557" s="1" t="s">
         <v>42</v>
@@ -16422,7 +16447,7 @@
         <v>552</v>
       </c>
       <c r="B558" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C558" s="1" t="s">
         <v>27</v>
@@ -16443,7 +16468,7 @@
         <v>553</v>
       </c>
       <c r="B559" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C559" s="12" t="s">
         <v>164</v>
@@ -16467,7 +16492,7 @@
         <v>554</v>
       </c>
       <c r="B560" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C560" s="12" t="s">
         <v>135</v>
@@ -16477,7 +16502,7 @@
       </c>
       <c r="F560" s="14"/>
       <c r="G560" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="I560" s="0" t="n">
         <f aca="false">IF(ISBLANK(B560),0,IF(D560="N/A",0,1))</f>
@@ -16494,7 +16519,7 @@
         <v>555</v>
       </c>
       <c r="B561" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C561" s="1" t="s">
         <v>56</v>
@@ -16515,7 +16540,7 @@
         <v>556</v>
       </c>
       <c r="B562" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C562" s="1" t="s">
         <v>22</v>
@@ -16524,7 +16549,7 @@
         <v>43</v>
       </c>
       <c r="G562" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="I562" s="0" t="n">
         <f aca="false">IF(ISBLANK(B562),0,IF(D562="N/A",0,1))</f>
@@ -16541,7 +16566,7 @@
         <v>557</v>
       </c>
       <c r="B563" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C563" s="1" t="s">
         <v>27</v>
@@ -16562,7 +16587,7 @@
         <v>558</v>
       </c>
       <c r="B564" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C564" s="1" t="s">
         <v>63</v>
@@ -16587,7 +16612,7 @@
         <v>559</v>
       </c>
       <c r="B565" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C565" s="1" t="s">
         <v>53</v>
@@ -16611,7 +16636,7 @@
         <v>560</v>
       </c>
       <c r="B566" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C566" s="1" t="s">
         <v>27</v>
@@ -16632,10 +16657,10 @@
         <v>561</v>
       </c>
       <c r="B567" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C567" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G567" s="1"/>
       <c r="H567" s="0" t="n">
@@ -16656,10 +16681,10 @@
         <v>562</v>
       </c>
       <c r="B568" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="C568" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="C568" s="1" t="s">
-        <v>638</v>
       </c>
       <c r="G568" s="1"/>
       <c r="H568" s="0" t="n">
@@ -16680,10 +16705,10 @@
         <v>563</v>
       </c>
       <c r="B569" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C569" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G569" s="1"/>
       <c r="H569" s="0" t="n">
@@ -16704,7 +16729,7 @@
         <v>564</v>
       </c>
       <c r="B570" s="2" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C570" s="12" t="s">
         <v>126</v>
@@ -16713,7 +16738,7 @@
         <v>43</v>
       </c>
       <c r="G570" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="I570" s="0" t="n">
         <f aca="false">IF(ISBLANK(B570),0,IF(D570="N/A",0,1))</f>
@@ -16730,7 +16755,7 @@
         <v>565</v>
       </c>
       <c r="B571" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C571" s="12" t="s">
         <v>126</v>
@@ -16739,7 +16764,7 @@
         <v>43</v>
       </c>
       <c r="G571" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="I571" s="0" t="n">
         <f aca="false">IF(ISBLANK(B571),0,IF(D571="N/A",0,1))</f>
@@ -16756,7 +16781,7 @@
         <v>566</v>
       </c>
       <c r="B572" s="2" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>166</v>
@@ -16780,10 +16805,13 @@
         <v>567</v>
       </c>
       <c r="B573" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="C573" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="D573" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="G573" s="1"/>
       <c r="H573" s="0" t="n">
@@ -16795,7 +16823,7 @@
       </c>
       <c r="J573" s="0" t="n">
         <f aca="false">IF(ISBLANK(D573),0,I573)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="574" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16804,7 +16832,7 @@
         <v>568</v>
       </c>
       <c r="B574" s="2" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C574" s="1" t="s">
         <v>104</v>
@@ -16828,7 +16856,7 @@
         <v>569</v>
       </c>
       <c r="B575" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C575" s="1" t="s">
         <v>104</v>
@@ -16852,7 +16880,7 @@
         <v>570</v>
       </c>
       <c r="B576" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C576" s="1" t="s">
         <v>468</v>
@@ -16876,7 +16904,7 @@
         <v>571</v>
       </c>
       <c r="B577" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C577" s="1" t="s">
         <v>104</v>
@@ -16900,7 +16928,7 @@
         <v>572</v>
       </c>
       <c r="B578" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C578" s="1" t="s">
         <v>47</v>
@@ -16924,7 +16952,7 @@
         <v>573</v>
       </c>
       <c r="B579" s="2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C579" s="1" t="s">
         <v>47</v>
@@ -16948,7 +16976,7 @@
         <v>574</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C580" s="1" t="s">
         <v>47</v>
@@ -16972,7 +17000,7 @@
         <v>575</v>
       </c>
       <c r="B581" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C581" s="1" t="s">
         <v>22</v>
@@ -16996,7 +17024,7 @@
         <v>576</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C582" s="12" t="s">
         <v>126</v>
@@ -17005,7 +17033,7 @@
         <v>43</v>
       </c>
       <c r="G582" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="I582" s="0" t="n">
         <f aca="false">IF(ISBLANK(B582),0,IF(D582="N/A",0,1))</f>
@@ -17022,7 +17050,7 @@
         <v>577</v>
       </c>
       <c r="B583" s="2" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C583" s="12" t="s">
         <v>126</v>
@@ -17031,7 +17059,7 @@
         <v>43</v>
       </c>
       <c r="G583" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="I583" s="0" t="n">
         <f aca="false">IF(ISBLANK(B583),0,IF(D583="N/A",0,1))</f>
@@ -17048,12 +17076,18 @@
         <v>578</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C584" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G584" s="1"/>
+      <c r="D584" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E584" s="22"/>
+      <c r="G584" s="1" t="s">
+        <v>659</v>
+      </c>
       <c r="H584" s="0" t="n">
         <v>110</v>
       </c>
@@ -17063,7 +17097,7 @@
       </c>
       <c r="J584" s="0" t="n">
         <f aca="false">IF(ISBLANK(D584),0,I584)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="585" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17072,7 +17106,7 @@
         <v>579</v>
       </c>
       <c r="B585" s="2" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="C585" s="1" t="s">
         <v>47</v>
@@ -17096,10 +17130,10 @@
         <v>580</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G586" s="1"/>
       <c r="H586" s="0" t="n">
@@ -17120,10 +17154,10 @@
         <v>581</v>
       </c>
       <c r="B587" s="2" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="C587" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G587" s="1"/>
       <c r="H587" s="0" t="n">
@@ -17144,10 +17178,10 @@
         <v>582</v>
       </c>
       <c r="B588" s="2" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="C588" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G588" s="1"/>
       <c r="H588" s="0" t="n">
@@ -17168,7 +17202,7 @@
         <v>583</v>
       </c>
       <c r="B589" s="2" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="C589" s="1" t="s">
         <v>47</v>
@@ -17192,10 +17226,13 @@
         <v>584</v>
       </c>
       <c r="B590" s="2" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="C590" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="D590" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="G590" s="1"/>
       <c r="H590" s="0" t="n">
@@ -17207,7 +17244,7 @@
       </c>
       <c r="J590" s="0" t="n">
         <f aca="false">IF(ISBLANK(D590),0,I590)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="591" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17216,7 +17253,7 @@
         <v>585</v>
       </c>
       <c r="B591" s="2" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="C591" s="1" t="s">
         <v>81</v>
@@ -17240,7 +17277,7 @@
         <v>586</v>
       </c>
       <c r="B592" s="2" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="C592" s="1" t="s">
         <v>12</v>
@@ -17264,7 +17301,7 @@
         <v>587</v>
       </c>
       <c r="B593" s="2" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="C593" s="1" t="s">
         <v>86</v>
@@ -17288,7 +17325,7 @@
         <v>588</v>
       </c>
       <c r="B594" s="2" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C594" s="1" t="s">
         <v>56</v>
@@ -17309,7 +17346,7 @@
         <v>589</v>
       </c>
       <c r="B595" s="2" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="C595" s="1" t="s">
         <v>56</v>
@@ -17330,7 +17367,7 @@
         <v>590</v>
       </c>
       <c r="B596" s="2" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="C596" s="1" t="s">
         <v>56</v>
@@ -17351,7 +17388,7 @@
         <v>591</v>
       </c>
       <c r="B597" s="2" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="C597" s="1" t="s">
         <v>56</v>
@@ -17372,7 +17409,7 @@
         <v>592</v>
       </c>
       <c r="B598" s="2" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="C598" s="1" t="s">
         <v>56</v>
@@ -17393,7 +17430,7 @@
         <v>593</v>
       </c>
       <c r="B599" s="2" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="C599" s="1" t="s">
         <v>47</v>
@@ -17417,7 +17454,7 @@
         <v>594</v>
       </c>
       <c r="B600" s="2" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C600" s="1" t="s">
         <v>22</v>
@@ -17441,7 +17478,7 @@
         <v>595</v>
       </c>
       <c r="B601" s="2" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="C601" s="1" t="s">
         <v>56</v>
@@ -17462,7 +17499,7 @@
         <v>596</v>
       </c>
       <c r="B602" s="2" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="C602" s="1" t="s">
         <v>42</v>
@@ -17486,7 +17523,7 @@
         <v>597</v>
       </c>
       <c r="B603" s="2" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="C603" s="1" t="s">
         <v>56</v>
@@ -17507,7 +17544,7 @@
         <v>598</v>
       </c>
       <c r="B604" s="2" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="C604" s="1" t="s">
         <v>148</v>
@@ -17528,7 +17565,7 @@
         <v>599</v>
       </c>
       <c r="B605" s="2" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="C605" s="1" t="s">
         <v>86</v>
@@ -17552,7 +17589,7 @@
         <v>600</v>
       </c>
       <c r="B606" s="2" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C606" s="1" t="s">
         <v>63</v>
@@ -17577,7 +17614,7 @@
         <v>601</v>
       </c>
       <c r="B607" s="2" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="C607" s="1" t="s">
         <v>27</v>
@@ -17598,7 +17635,7 @@
         <v>602</v>
       </c>
       <c r="B608" s="2" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C608" s="1" t="s">
         <v>86</v>
@@ -17622,7 +17659,7 @@
         <v>603</v>
       </c>
       <c r="B609" s="2" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="C609" s="1" t="s">
         <v>27</v>
@@ -17643,7 +17680,7 @@
         <v>604</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C610" s="1" t="s">
         <v>22</v>
@@ -17667,7 +17704,7 @@
         <v>605</v>
       </c>
       <c r="B611" s="2" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C611" s="1" t="s">
         <v>27</v>
@@ -17688,7 +17725,7 @@
         <v>606</v>
       </c>
       <c r="B612" s="2" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C612" s="1" t="s">
         <v>218</v>
@@ -17709,7 +17746,7 @@
         <v>607</v>
       </c>
       <c r="B613" s="2" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="C613" s="1" t="s">
         <v>27</v>
@@ -17730,7 +17767,7 @@
         <v>608</v>
       </c>
       <c r="B614" s="2" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C614" s="1" t="s">
         <v>27</v>
@@ -17751,7 +17788,7 @@
         <v>609</v>
       </c>
       <c r="B615" s="2" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="C615" s="1" t="s">
         <v>16</v>
@@ -17776,7 +17813,7 @@
         <v>610</v>
       </c>
       <c r="B616" s="2" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="C616" s="1" t="s">
         <v>56</v>
@@ -17797,7 +17834,7 @@
         <v>611</v>
       </c>
       <c r="B617" s="2" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C617" s="1" t="s">
         <v>27</v>
@@ -17818,7 +17855,7 @@
         <v>612</v>
       </c>
       <c r="B618" s="2" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="C618" s="1" t="s">
         <v>27</v>
@@ -17839,7 +17876,7 @@
         <v>613</v>
       </c>
       <c r="B619" s="2" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="C619" s="1" t="s">
         <v>89</v>
@@ -17863,7 +17900,7 @@
         <v>614</v>
       </c>
       <c r="B620" s="2" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C620" s="1" t="s">
         <v>27</v>
@@ -17884,7 +17921,7 @@
         <v>615</v>
       </c>
       <c r="B621" s="2" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C621" s="1" t="s">
         <v>89</v>
@@ -17908,7 +17945,7 @@
         <v>616</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="C622" s="1" t="s">
         <v>42</v>
@@ -17932,7 +17969,7 @@
         <v>617</v>
       </c>
       <c r="B623" s="2" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="C623" s="12" t="s">
         <v>135</v>
@@ -17942,7 +17979,7 @@
       </c>
       <c r="F623" s="13"/>
       <c r="G623" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="I623" s="0" t="n">
         <f aca="false">IF(ISBLANK(B623),0,IF(D623="N/A",0,1))</f>
@@ -17959,7 +17996,7 @@
         <v>618</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C624" s="12" t="s">
         <v>126</v>
@@ -17968,7 +18005,7 @@
         <v>43</v>
       </c>
       <c r="G624" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="I624" s="0" t="n">
         <f aca="false">IF(ISBLANK(B624),0,IF(D624="N/A",0,1))</f>
@@ -17985,7 +18022,7 @@
         <v>619</v>
       </c>
       <c r="B625" s="2" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="C625" s="12" t="s">
         <v>126</v>
@@ -17994,7 +18031,7 @@
         <v>43</v>
       </c>
       <c r="G625" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="I625" s="0" t="n">
         <f aca="false">IF(ISBLANK(B625),0,IF(D625="N/A",0,1))</f>
@@ -18011,7 +18048,7 @@
         <v>620</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C626" s="1" t="s">
         <v>56</v>
@@ -18032,7 +18069,7 @@
         <v>621</v>
       </c>
       <c r="B627" s="2" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="C627" s="1" t="s">
         <v>42</v>
@@ -18056,7 +18093,7 @@
         <v>622</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C628" s="1" t="s">
         <v>47</v>
@@ -18080,7 +18117,7 @@
         <v>623</v>
       </c>
       <c r="B629" s="2" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C629" s="1" t="s">
         <v>468</v>
@@ -18104,7 +18141,7 @@
         <v>624</v>
       </c>
       <c r="B630" s="2" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C630" s="1" t="s">
         <v>468</v>
@@ -18128,7 +18165,7 @@
         <v>625</v>
       </c>
       <c r="B631" s="2" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C631" s="1" t="s">
         <v>53</v>
@@ -18152,7 +18189,7 @@
         <v>626</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C632" s="1" t="s">
         <v>27</v>
@@ -18173,7 +18210,7 @@
         <v>627</v>
       </c>
       <c r="B633" s="2" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C633" s="1" t="s">
         <v>63</v>
@@ -18198,7 +18235,7 @@
         <v>628</v>
       </c>
       <c r="B634" s="2" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="C634" s="1" t="s">
         <v>22</v>
@@ -18224,7 +18261,7 @@
         <v>629</v>
       </c>
       <c r="B635" s="2" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C635" s="1" t="s">
         <v>12</v>
@@ -18248,7 +18285,7 @@
         <v>630</v>
       </c>
       <c r="B636" s="2" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="C636" s="12" t="s">
         <v>126</v>
@@ -18257,7 +18294,7 @@
         <v>43</v>
       </c>
       <c r="G636" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="I636" s="0" t="n">
         <f aca="false">IF(ISBLANK(B636),0,IF(D636="N/A",0,1))</f>
@@ -18274,7 +18311,7 @@
         <v>631</v>
       </c>
       <c r="B637" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="C637" s="1" t="s">
         <v>47</v>
@@ -18298,7 +18335,7 @@
         <v>632</v>
       </c>
       <c r="B638" s="2" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C638" s="12" t="s">
         <v>126</v>
@@ -18307,7 +18344,7 @@
         <v>43</v>
       </c>
       <c r="G638" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="I638" s="0" t="n">
         <f aca="false">IF(ISBLANK(B638),0,IF(D638="N/A",0,1))</f>
@@ -18324,7 +18361,7 @@
         <v>633</v>
       </c>
       <c r="B639" s="2" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C639" s="1" t="s">
         <v>86</v>
@@ -18348,7 +18385,7 @@
         <v>634</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C640" s="12" t="s">
         <v>173</v>
@@ -18373,7 +18410,7 @@
         <v>635</v>
       </c>
       <c r="B641" s="2" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C641" s="12" t="s">
         <v>164</v>
@@ -18397,7 +18434,7 @@
         <v>636</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C642" s="1" t="s">
         <v>22</v>
@@ -18421,7 +18458,7 @@
         <v>637</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C643" s="12" t="s">
         <v>164</v>
@@ -18445,7 +18482,7 @@
         <v>638</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C644" s="1" t="s">
         <v>42</v>
@@ -18466,7 +18503,7 @@
         <v>639</v>
       </c>
       <c r="B645" s="2" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C645" s="1" t="s">
         <v>86</v>
@@ -18490,7 +18527,7 @@
         <v>640</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C646" s="1" t="s">
         <v>42</v>
@@ -18514,7 +18551,7 @@
         <v>641</v>
       </c>
       <c r="B647" s="2" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C647" s="1" t="s">
         <v>42</v>
@@ -18538,7 +18575,7 @@
         <v>642</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="C648" s="1" t="s">
         <v>42</v>
@@ -18562,7 +18599,7 @@
         <v>643</v>
       </c>
       <c r="B649" s="2" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C649" s="1" t="s">
         <v>42</v>
@@ -18586,7 +18623,7 @@
         <v>644</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C650" s="1" t="s">
         <v>42</v>
@@ -18610,7 +18647,7 @@
         <v>645</v>
       </c>
       <c r="B651" s="2" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="C651" s="1" t="s">
         <v>86</v>
@@ -18634,7 +18671,7 @@
         <v>646</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C652" s="1" t="s">
         <v>22</v>
@@ -18658,7 +18695,7 @@
         <v>647</v>
       </c>
       <c r="B653" s="2" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="C653" s="1" t="s">
         <v>22</v>
@@ -18668,7 +18705,7 @@
       </c>
       <c r="F653" s="13"/>
       <c r="G653" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="I653" s="0" t="n">
         <f aca="false">IF(ISBLANK(B653),0,IF(D653="N/A",0,1))</f>
@@ -18685,7 +18722,7 @@
         <v>648</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="C654" s="1" t="s">
         <v>27</v>
@@ -18706,7 +18743,7 @@
         <v>649</v>
       </c>
       <c r="B655" s="2" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C655" s="1" t="s">
         <v>27</v>
@@ -18727,7 +18764,7 @@
         <v>650</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="C656" s="1" t="s">
         <v>148</v>
@@ -18748,7 +18785,7 @@
         <v>651</v>
       </c>
       <c r="B657" s="2" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="C657" s="1" t="s">
         <v>22</v>
@@ -18773,7 +18810,7 @@
         <v>652</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="C658" s="1" t="s">
         <v>63</v>
@@ -18798,7 +18835,7 @@
         <v>653</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="C659" s="1" t="s">
         <v>27</v>
@@ -18819,7 +18856,7 @@
         <v>654</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C660" s="1" t="s">
         <v>27</v>
@@ -18840,7 +18877,7 @@
         <v>655</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C661" s="12" t="s">
         <v>126</v>
@@ -18865,7 +18902,7 @@
         <v>656</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C662" s="12" t="s">
         <v>135</v>
@@ -18875,7 +18912,7 @@
       </c>
       <c r="F662" s="14"/>
       <c r="G662" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="I662" s="0" t="n">
         <f aca="false">IF(ISBLANK(B662),0,IF(D662="N/A",0,1))</f>
@@ -18892,7 +18929,7 @@
         <v>657</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C663" s="1" t="s">
         <v>27</v>
@@ -18913,7 +18950,7 @@
         <v>658</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C664" s="1" t="s">
         <v>16</v>
@@ -18937,7 +18974,7 @@
         <v>659</v>
       </c>
       <c r="B665" s="2" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C665" s="1" t="s">
         <v>47</v>
@@ -18961,7 +18998,7 @@
         <v>660</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="C666" s="1" t="s">
         <v>47</v>
@@ -18985,7 +19022,7 @@
         <v>661</v>
       </c>
       <c r="B667" s="2" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="C667" s="1" t="s">
         <v>104</v>
@@ -19009,7 +19046,7 @@
         <v>662</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="C668" s="1" t="s">
         <v>47</v>
@@ -19033,7 +19070,7 @@
         <v>663</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="C669" s="1" t="s">
         <v>81</v>
@@ -19057,7 +19094,7 @@
         <v>664</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="C670" s="1" t="s">
         <v>27</v>
@@ -19078,7 +19115,7 @@
         <v>665</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="C671" s="1" t="s">
         <v>27</v>
@@ -19099,7 +19136,7 @@
         <v>666</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="C672" s="1" t="s">
         <v>27</v>
@@ -19120,7 +19157,7 @@
         <v>667</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="C673" s="12" t="s">
         <v>135</v>
@@ -19145,7 +19182,7 @@
         <v>668</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C674" s="1" t="s">
         <v>89</v>
@@ -19169,7 +19206,7 @@
         <v>669</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="C675" s="1" t="s">
         <v>27</v>
@@ -19190,7 +19227,7 @@
         <v>670</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C676" s="1" t="s">
         <v>27</v>
@@ -19211,7 +19248,7 @@
         <v>671</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C677" s="1" t="s">
         <v>27</v>
@@ -19232,7 +19269,7 @@
         <v>672</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="C678" s="1" t="s">
         <v>89</v>
@@ -19256,7 +19293,7 @@
         <v>673</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C679" s="1" t="s">
         <v>27</v>
@@ -19277,7 +19314,7 @@
         <v>674</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C680" s="1" t="s">
         <v>27</v>
@@ -19298,7 +19335,7 @@
         <v>675</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C681" s="1" t="s">
         <v>27</v>
@@ -19319,7 +19356,7 @@
         <v>676</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="C682" s="1" t="s">
         <v>27</v>
@@ -19340,7 +19377,7 @@
         <v>677</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C683" s="1" t="s">
         <v>218</v>
@@ -19349,7 +19386,7 @@
         <v>43</v>
       </c>
       <c r="G683" s="1" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="I683" s="0" t="n">
         <f aca="false">IF(ISBLANK(B683),0,IF(D683="N/A",0,1))</f>
@@ -19366,7 +19403,7 @@
         <v>678</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="C684" s="1" t="s">
         <v>53</v>
@@ -19390,7 +19427,7 @@
         <v>679</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="C685" s="1" t="s">
         <v>22</v>
@@ -19414,7 +19451,7 @@
         <v>680</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C686" s="1" t="s">
         <v>27</v>
@@ -19435,7 +19472,7 @@
         <v>681</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C687" s="1" t="s">
         <v>56</v>
@@ -19456,7 +19493,7 @@
         <v>682</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C688" s="12" t="s">
         <v>164</v>
@@ -19480,7 +19517,7 @@
         <v>683</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="C689" s="1" t="s">
         <v>22</v>
@@ -19504,7 +19541,7 @@
         <v>684</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C690" s="1" t="s">
         <v>50</v>
@@ -19528,7 +19565,7 @@
         <v>685</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C691" s="1" t="s">
         <v>218</v>
@@ -19537,7 +19574,7 @@
         <v>43</v>
       </c>
       <c r="G691" s="1" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="I691" s="0" t="n">
         <f aca="false">IF(ISBLANK(B691),0,IF(D691="N/A",0,1))</f>
@@ -19554,7 +19591,7 @@
         <v>686</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="C692" s="1" t="s">
         <v>27</v>
@@ -19575,7 +19612,7 @@
         <v>687</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="C693" s="1" t="s">
         <v>56</v>
@@ -19596,7 +19633,7 @@
         <v>688</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="C694" s="1" t="s">
         <v>53</v>
@@ -19623,7 +19660,7 @@
         <v>689</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="C695" s="1" t="s">
         <v>148</v>
@@ -19644,7 +19681,7 @@
         <v>690</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="C696" s="1" t="s">
         <v>47</v>
@@ -19668,7 +19705,7 @@
         <v>691</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="C697" s="1" t="s">
         <v>47</v>
@@ -19692,7 +19729,7 @@
         <v>692</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="C698" s="1" t="s">
         <v>86</v>
@@ -19716,7 +19753,7 @@
         <v>693</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="C699" s="1" t="s">
         <v>27</v>
@@ -19737,7 +19774,7 @@
         <v>694</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="C700" s="1" t="s">
         <v>27</v>
@@ -19758,7 +19795,7 @@
         <v>695</v>
       </c>
       <c r="B701" s="2" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C701" s="1" t="s">
         <v>53</v>
@@ -19782,7 +19819,7 @@
         <v>696</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C702" s="1" t="s">
         <v>27</v>
@@ -19803,7 +19840,7 @@
         <v>697</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C703" s="1" t="s">
         <v>27</v>
@@ -19824,7 +19861,7 @@
         <v>698</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C704" s="1" t="s">
         <v>47</v>
@@ -19848,7 +19885,7 @@
         <v>699</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C705" s="1" t="s">
         <v>166</v>
@@ -19872,7 +19909,7 @@
         <v>700</v>
       </c>
       <c r="B706" s="2" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="C706" s="1" t="s">
         <v>27</v>
@@ -19893,7 +19930,7 @@
         <v>701</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C707" s="1" t="s">
         <v>56</v>
@@ -19914,7 +19951,7 @@
         <v>702</v>
       </c>
       <c r="B708" s="2" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="C708" s="1" t="s">
         <v>27</v>
@@ -19935,7 +19972,7 @@
         <v>703</v>
       </c>
       <c r="B709" s="2" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="C709" s="1" t="s">
         <v>50</v>
@@ -19959,7 +19996,7 @@
         <v>704</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="C710" s="1" t="s">
         <v>42</v>
@@ -19983,7 +20020,7 @@
         <v>705</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C711" s="1" t="s">
         <v>53</v>
@@ -20007,7 +20044,7 @@
         <v>706</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C712" s="1" t="s">
         <v>99</v>
@@ -20028,7 +20065,7 @@
         <v>707</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C713" s="1" t="s">
         <v>99</v>
@@ -20049,7 +20086,7 @@
         <v>708</v>
       </c>
       <c r="B714" s="2" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="C714" s="1" t="s">
         <v>99</v>
@@ -20070,7 +20107,7 @@
         <v>709</v>
       </c>
       <c r="B715" s="2" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="C715" s="1" t="s">
         <v>22</v>
@@ -20080,7 +20117,7 @@
       </c>
       <c r="F715" s="13"/>
       <c r="G715" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="I715" s="0" t="n">
         <f aca="false">IF(ISBLANK(B715),0,IF(D715="N/A",0,1))</f>
@@ -20097,7 +20134,7 @@
         <v>710</v>
       </c>
       <c r="B716" s="2" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="C716" s="12" t="s">
         <v>25</v>
@@ -20122,7 +20159,7 @@
         <v>711</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C717" s="12" t="s">
         <v>25</v>
@@ -20147,7 +20184,7 @@
         <v>712</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="C718" s="1" t="s">
         <v>81</v>
@@ -20171,7 +20208,7 @@
         <v>713</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C719" s="1" t="s">
         <v>42</v>
@@ -20192,7 +20229,7 @@
         <v>714</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="C720" s="1" t="s">
         <v>27</v>
@@ -20213,7 +20250,7 @@
         <v>715</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C721" s="1" t="s">
         <v>42</v>
@@ -20237,7 +20274,7 @@
         <v>716</v>
       </c>
       <c r="B722" s="2" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C722" s="1" t="s">
         <v>104</v>
@@ -20261,7 +20298,7 @@
         <v>717</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="C723" s="1" t="s">
         <v>104</v>
@@ -20285,7 +20322,7 @@
         <v>718</v>
       </c>
       <c r="B724" s="2" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="C724" s="12" t="s">
         <v>164</v>
@@ -20309,7 +20346,7 @@
         <v>719</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C725" s="15" t="s">
         <v>183</v>
@@ -20333,7 +20370,7 @@
         <v>720</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C726" s="1" t="s">
         <v>148</v>
@@ -20354,7 +20391,7 @@
         <v>721</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="C727" s="1" t="s">
         <v>148</v>
@@ -20375,7 +20412,7 @@
         <v>722</v>
       </c>
       <c r="B728" s="2" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C728" s="1" t="s">
         <v>148</v>
@@ -20396,7 +20433,7 @@
         <v>723</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="C729" s="1" t="s">
         <v>148</v>
@@ -20417,7 +20454,7 @@
         <v>724</v>
       </c>
       <c r="B730" s="2" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="C730" s="12" t="s">
         <v>25</v>
@@ -20442,7 +20479,7 @@
         <v>725</v>
       </c>
       <c r="B731" s="2" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C731" s="1" t="s">
         <v>47</v>
@@ -20466,7 +20503,7 @@
         <v>726</v>
       </c>
       <c r="B732" s="2" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="C732" s="1" t="s">
         <v>47</v>
@@ -20490,7 +20527,7 @@
         <v>727</v>
       </c>
       <c r="B733" s="2" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="C733" s="1" t="s">
         <v>148</v>
@@ -20511,7 +20548,7 @@
         <v>728</v>
       </c>
       <c r="B734" s="2" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="C734" s="1" t="s">
         <v>42</v>
@@ -20535,7 +20572,7 @@
         <v>729</v>
       </c>
       <c r="B735" s="2" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="C735" s="1" t="s">
         <v>22</v>
@@ -20556,7 +20593,7 @@
         <v>730</v>
       </c>
       <c r="B736" s="2" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C736" s="1" t="s">
         <v>22</v>
@@ -20580,7 +20617,7 @@
         <v>731</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="C737" s="1" t="s">
         <v>22</v>
@@ -20601,7 +20638,7 @@
         <v>732</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C738" s="1" t="s">
         <v>22</v>
@@ -20622,7 +20659,7 @@
         <v>733</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="C739" s="1" t="s">
         <v>27</v>
@@ -20643,7 +20680,7 @@
         <v>734</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="C740" s="1" t="s">
         <v>42</v>
@@ -20653,7 +20690,7 @@
       </c>
       <c r="F740" s="13"/>
       <c r="G740" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="I740" s="0" t="n">
         <f aca="false">IF(ISBLANK(B740),0,IF(D740="N/A",0,1))</f>
@@ -20670,7 +20707,7 @@
         <v>735</v>
       </c>
       <c r="B741" s="2" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="C741" s="1" t="s">
         <v>53</v>
@@ -20680,7 +20717,7 @@
       </c>
       <c r="F741" s="22"/>
       <c r="G741" s="1" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="I741" s="0" t="n">
         <f aca="false">IF(ISBLANK(B741),0,IF(D741="N/A",0,1))</f>
@@ -20697,7 +20734,7 @@
         <v>736</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C742" s="12" t="s">
         <v>164</v>
@@ -20721,7 +20758,7 @@
         <v>737</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C743" s="1" t="s">
         <v>56</v>
@@ -20742,7 +20779,7 @@
         <v>738</v>
       </c>
       <c r="B744" s="2" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="C744" s="1" t="s">
         <v>81</v>
@@ -20766,7 +20803,7 @@
         <v>739</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="C745" s="1" t="s">
         <v>148</v>
@@ -20787,7 +20824,7 @@
         <v>740</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="C746" s="1" t="s">
         <v>86</v>
@@ -20811,7 +20848,7 @@
         <v>741</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="C747" s="1" t="s">
         <v>86</v>
@@ -20835,10 +20872,10 @@
         <v>742</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="C748" s="1" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="G748" s="1"/>
       <c r="I748" s="0" t="n">
@@ -20856,7 +20893,7 @@
         <v>743</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C749" s="15" t="s">
         <v>101</v>
@@ -20880,7 +20917,7 @@
         <v>744</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="C750" s="1" t="s">
         <v>166</v>
@@ -20904,7 +20941,7 @@
         <v>745</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C751" s="1" t="s">
         <v>86</v>
@@ -20928,7 +20965,7 @@
         <v>746</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C752" s="1" t="s">
         <v>27</v>
@@ -20949,7 +20986,7 @@
         <v>747</v>
       </c>
       <c r="B753" s="2" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="C753" s="1" t="s">
         <v>86</v>
@@ -20973,7 +21010,7 @@
         <v>748</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C754" s="1" t="s">
         <v>56</v>
@@ -20994,7 +21031,7 @@
         <v>749</v>
       </c>
       <c r="B755" s="2" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="C755" s="1" t="s">
         <v>12</v>
@@ -21018,7 +21055,7 @@
         <v>750</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C756" s="1" t="s">
         <v>86</v>
@@ -21042,7 +21079,7 @@
         <v>751</v>
       </c>
       <c r="B757" s="2" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="C757" s="1" t="s">
         <v>86</v>
@@ -21066,7 +21103,7 @@
         <v>752</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="C758" s="1" t="s">
         <v>56</v>
@@ -21087,7 +21124,7 @@
         <v>753</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C759" s="1" t="s">
         <v>56</v>
@@ -21108,7 +21145,7 @@
         <v>754</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="C760" s="1" t="s">
         <v>148</v>
@@ -21129,7 +21166,7 @@
         <v>755</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C761" s="1" t="s">
         <v>56</v>
@@ -21150,7 +21187,7 @@
         <v>756</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="C762" s="1" t="s">
         <v>56</v>
@@ -21171,7 +21208,7 @@
         <v>757</v>
       </c>
       <c r="B763" s="2" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="C763" s="1" t="s">
         <v>56</v>
@@ -21192,7 +21229,7 @@
         <v>758</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="C764" s="1" t="s">
         <v>56</v>
@@ -21213,7 +21250,7 @@
         <v>759</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="C765" s="1" t="s">
         <v>27</v>
@@ -21234,7 +21271,7 @@
         <v>760</v>
       </c>
       <c r="B766" s="2" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="C766" s="1" t="s">
         <v>218</v>
@@ -21255,7 +21292,7 @@
         <v>761</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="C767" s="1" t="s">
         <v>56</v>
@@ -21276,7 +21313,7 @@
         <v>762</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="C768" s="1" t="s">
         <v>63</v>
@@ -21301,7 +21338,7 @@
         <v>763</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="C769" s="1" t="s">
         <v>79</v>
@@ -21325,7 +21362,7 @@
         <v>764</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="C770" s="1" t="s">
         <v>63</v>
@@ -21335,7 +21372,7 @@
       </c>
       <c r="F770" s="13"/>
       <c r="G770" s="1" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="I770" s="0" t="n">
         <f aca="false">IF(ISBLANK(B770),0,IF(D770="N/A",0,1))</f>
@@ -21352,7 +21389,7 @@
         <v>765</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="C771" s="1" t="s">
         <v>27</v>
@@ -21373,7 +21410,7 @@
         <v>766</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="C772" s="1" t="s">
         <v>27</v>
@@ -21394,7 +21431,7 @@
         <v>767</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C773" s="1" t="s">
         <v>27</v>
@@ -21415,7 +21452,7 @@
         <v>768</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="C774" s="1" t="s">
         <v>148</v>
@@ -21436,7 +21473,7 @@
         <v>769</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="C775" s="1" t="s">
         <v>63</v>
@@ -21446,7 +21483,7 @@
       </c>
       <c r="F775" s="13"/>
       <c r="G775" s="1" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="I775" s="0" t="n">
         <f aca="false">IF(ISBLANK(B775),0,IF(D775="N/A",0,1))</f>
@@ -21463,7 +21500,7 @@
         <v>770</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C776" s="1" t="s">
         <v>148</v>
@@ -21484,7 +21521,7 @@
         <v>771</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="C777" s="1" t="s">
         <v>148</v>
@@ -21505,7 +21542,7 @@
         <v>772</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="C778" s="1" t="s">
         <v>148</v>
@@ -21526,7 +21563,7 @@
         <v>773</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="C779" s="1" t="s">
         <v>148</v>
@@ -21547,7 +21584,7 @@
         <v>774</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="C780" s="1" t="s">
         <v>148</v>
@@ -21568,7 +21605,7 @@
         <v>775</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="C781" s="1" t="s">
         <v>148</v>
@@ -21589,7 +21626,7 @@
         <v>776</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="C782" s="1" t="s">
         <v>148</v>
@@ -21610,7 +21647,7 @@
         <v>777</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="C783" s="1" t="s">
         <v>148</v>
@@ -21631,13 +21668,13 @@
         <v>778</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="C784" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D784" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G784" s="1"/>
       <c r="I784" s="0" t="n">
@@ -21655,13 +21692,13 @@
         <v>779</v>
       </c>
       <c r="B785" s="2" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="C785" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D785" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G785" s="1"/>
       <c r="I785" s="0" t="n">
@@ -21679,13 +21716,13 @@
         <v>780</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="C786" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D786" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G786" s="1"/>
       <c r="I786" s="0" t="n">
@@ -21703,13 +21740,13 @@
         <v>781</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="C787" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D787" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G787" s="1"/>
       <c r="I787" s="0" t="n">
@@ -21727,13 +21764,13 @@
         <v>782</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="C788" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D788" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G788" s="1"/>
       <c r="I788" s="0" t="n">
@@ -21751,13 +21788,13 @@
         <v>783</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="C789" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D789" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G789" s="1"/>
       <c r="I789" s="0" t="n">
@@ -21775,13 +21812,13 @@
         <v>784</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="C790" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D790" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G790" s="1"/>
       <c r="I790" s="0" t="n">
@@ -21799,13 +21836,13 @@
         <v>785</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="C791" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D791" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G791" s="1"/>
       <c r="I791" s="0" t="n">
@@ -21823,13 +21860,13 @@
         <v>786</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C792" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D792" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G792" s="1"/>
       <c r="I792" s="0" t="n">
@@ -21847,13 +21884,13 @@
         <v>787</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="C793" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D793" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G793" s="1"/>
       <c r="I793" s="0" t="n">
@@ -21871,13 +21908,13 @@
         <v>788</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="C794" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D794" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G794" s="1"/>
       <c r="I794" s="0" t="n">
@@ -21895,13 +21932,13 @@
         <v>789</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D795" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G795" s="1"/>
       <c r="I795" s="0" t="n">
@@ -21919,13 +21956,13 @@
         <v>790</v>
       </c>
       <c r="B796" s="2" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="C796" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D796" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G796" s="1"/>
       <c r="I796" s="0" t="n">
@@ -21943,13 +21980,13 @@
         <v>791</v>
       </c>
       <c r="B797" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="C797" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="C797" s="1" t="s">
-        <v>879</v>
-      </c>
       <c r="D797" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G797" s="1"/>
       <c r="I797" s="0" t="n">
@@ -21967,13 +22004,13 @@
         <v>792</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D798" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G798" s="1"/>
       <c r="I798" s="0" t="n">
@@ -21991,13 +22028,13 @@
         <v>793</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D799" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G799" s="1"/>
       <c r="I799" s="0" t="n">
@@ -22015,13 +22052,13 @@
         <v>794</v>
       </c>
       <c r="B800" s="2" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D800" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G800" s="1"/>
       <c r="I800" s="0" t="n">
@@ -22039,13 +22076,13 @@
         <v>795</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D801" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G801" s="1"/>
       <c r="I801" s="0" t="n">
@@ -22063,13 +22100,13 @@
         <v>796</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="C802" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D802" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G802" s="1"/>
       <c r="I802" s="0" t="n">
@@ -22087,13 +22124,13 @@
         <v>797</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="C803" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D803" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G803" s="1"/>
       <c r="I803" s="0" t="n">
@@ -22111,13 +22148,13 @@
         <v>798</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="C804" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D804" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G804" s="1"/>
       <c r="I804" s="0" t="n">
@@ -22135,13 +22172,13 @@
         <v>799</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C805" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D805" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G805" s="1"/>
       <c r="I805" s="0" t="n">
@@ -22159,13 +22196,13 @@
         <v>800</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="C806" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D806" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G806" s="1"/>
       <c r="I806" s="0" t="n">
@@ -22183,13 +22220,13 @@
         <v>801</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="C807" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D807" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G807" s="1"/>
       <c r="I807" s="0" t="n">
@@ -22207,13 +22244,13 @@
         <v>802</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D808" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G808" s="1"/>
       <c r="I808" s="0" t="n">
@@ -22231,13 +22268,13 @@
         <v>803</v>
       </c>
       <c r="B809" s="2" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D809" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G809" s="1"/>
       <c r="I809" s="0" t="n">
@@ -22255,13 +22292,13 @@
         <v>804</v>
       </c>
       <c r="B810" s="2" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D810" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G810" s="1"/>
       <c r="I810" s="0" t="n">
@@ -22279,13 +22316,13 @@
         <v>805</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D811" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G811" s="1"/>
       <c r="I811" s="0" t="n">
@@ -22303,13 +22340,13 @@
         <v>806</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D812" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G812" s="1"/>
       <c r="I812" s="0" t="n">
@@ -22327,13 +22364,13 @@
         <v>807</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D813" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G813" s="1"/>
       <c r="I813" s="0" t="n">
@@ -22351,13 +22388,13 @@
         <v>808</v>
       </c>
       <c r="B814" s="2" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D814" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G814" s="1"/>
       <c r="I814" s="0" t="n">
@@ -22375,13 +22412,13 @@
         <v>809</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D815" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G815" s="1"/>
       <c r="I815" s="0" t="n">
@@ -22399,13 +22436,13 @@
         <v>810</v>
       </c>
       <c r="B816" s="2" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D816" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G816" s="1"/>
       <c r="I816" s="0" t="n">
@@ -22423,13 +22460,13 @@
         <v>811</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D817" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G817" s="1"/>
       <c r="I817" s="0" t="n">
@@ -22447,13 +22484,13 @@
         <v>812</v>
       </c>
       <c r="B818" s="2" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D818" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G818" s="1"/>
       <c r="I818" s="0" t="n">
@@ -22471,13 +22508,13 @@
         <v>813</v>
       </c>
       <c r="B819" s="2" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D819" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G819" s="1"/>
       <c r="I819" s="0" t="n">
@@ -22495,13 +22532,13 @@
         <v>814</v>
       </c>
       <c r="B820" s="2" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D820" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G820" s="1"/>
       <c r="I820" s="0" t="n">
@@ -22519,13 +22556,13 @@
         <v>815</v>
       </c>
       <c r="B821" s="2" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D821" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G821" s="1"/>
       <c r="I821" s="0" t="n">
@@ -22543,13 +22580,13 @@
         <v>816</v>
       </c>
       <c r="B822" s="2" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D822" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G822" s="1"/>
       <c r="I822" s="0" t="n">
@@ -22567,13 +22604,13 @@
         <v>817</v>
       </c>
       <c r="B823" s="2" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C823" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D823" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G823" s="1"/>
       <c r="I823" s="0" t="n">
@@ -22591,13 +22628,13 @@
         <v>818</v>
       </c>
       <c r="B824" s="2" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C824" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D824" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G824" s="1"/>
       <c r="I824" s="0" t="n">
@@ -22615,13 +22652,13 @@
         <v>819</v>
       </c>
       <c r="B825" s="2" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="C825" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D825" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G825" s="1"/>
       <c r="I825" s="0" t="n">
@@ -22639,13 +22676,13 @@
         <v>820</v>
       </c>
       <c r="B826" s="2" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D826" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G826" s="1"/>
       <c r="I826" s="0" t="n">
@@ -22663,13 +22700,13 @@
         <v>821</v>
       </c>
       <c r="B827" s="2" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="C827" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D827" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G827" s="1"/>
       <c r="I827" s="0" t="n">
@@ -22687,13 +22724,13 @@
         <v>822</v>
       </c>
       <c r="B828" s="2" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="C828" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D828" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G828" s="1"/>
       <c r="I828" s="0" t="n">
@@ -22711,13 +22748,13 @@
         <v>823</v>
       </c>
       <c r="B829" s="2" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="C829" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D829" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G829" s="1"/>
       <c r="I829" s="0" t="n">
@@ -22735,13 +22772,13 @@
         <v>824</v>
       </c>
       <c r="B830" s="2" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C830" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D830" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G830" s="1"/>
       <c r="I830" s="0" t="n">
@@ -22759,13 +22796,13 @@
         <v>825</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="C831" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D831" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G831" s="1"/>
       <c r="I831" s="0" t="n">
@@ -22783,13 +22820,13 @@
         <v>826</v>
       </c>
       <c r="B832" s="2" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C832" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D832" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G832" s="1"/>
       <c r="I832" s="0" t="n">
@@ -22807,13 +22844,13 @@
         <v>827</v>
       </c>
       <c r="B833" s="2" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="C833" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D833" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G833" s="1"/>
       <c r="I833" s="0" t="n">
@@ -22831,13 +22868,13 @@
         <v>828</v>
       </c>
       <c r="B834" s="2" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="C834" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D834" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G834" s="1"/>
       <c r="I834" s="0" t="n">
@@ -22855,13 +22892,13 @@
         <v>829</v>
       </c>
       <c r="B835" s="2" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="C835" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D835" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G835" s="1"/>
       <c r="I835" s="0" t="n">
@@ -22879,13 +22916,13 @@
         <v>830</v>
       </c>
       <c r="B836" s="2" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C836" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D836" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G836" s="1"/>
       <c r="I836" s="0" t="n">
@@ -22903,13 +22940,13 @@
         <v>831</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="C837" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D837" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G837" s="1"/>
       <c r="I837" s="0" t="n">
@@ -22927,13 +22964,13 @@
         <v>832</v>
       </c>
       <c r="B838" s="2" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="C838" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D838" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G838" s="1"/>
       <c r="I838" s="0" t="n">
@@ -22951,13 +22988,13 @@
         <v>833</v>
       </c>
       <c r="B839" s="2" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="C839" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D839" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G839" s="1"/>
       <c r="I839" s="0" t="n">
@@ -22975,13 +23012,13 @@
         <v>834</v>
       </c>
       <c r="B840" s="2" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="C840" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D840" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G840" s="1"/>
       <c r="I840" s="0" t="n">
@@ -22999,13 +23036,13 @@
         <v>835</v>
       </c>
       <c r="B841" s="2" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C841" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D841" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G841" s="1"/>
       <c r="I841" s="0" t="n">
@@ -23023,13 +23060,13 @@
         <v>836</v>
       </c>
       <c r="B842" s="2" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="C842" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D842" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G842" s="1"/>
       <c r="I842" s="0" t="n">
@@ -23047,13 +23084,13 @@
         <v>837</v>
       </c>
       <c r="B843" s="2" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="C843" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D843" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G843" s="1"/>
       <c r="I843" s="0" t="n">
@@ -23071,13 +23108,13 @@
         <v>838</v>
       </c>
       <c r="B844" s="2" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="C844" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D844" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G844" s="1"/>
       <c r="I844" s="0" t="n">
@@ -23095,13 +23132,13 @@
         <v>839</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="C845" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D845" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G845" s="1"/>
       <c r="I845" s="0" t="n">
@@ -23119,13 +23156,13 @@
         <v>840</v>
       </c>
       <c r="B846" s="2" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C846" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D846" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G846" s="1"/>
       <c r="I846" s="0" t="n">
@@ -23143,13 +23180,13 @@
         <v>841</v>
       </c>
       <c r="B847" s="2" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="C847" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D847" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G847" s="1"/>
       <c r="I847" s="0" t="n">
@@ -23167,13 +23204,13 @@
         <v>842</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="C848" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D848" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G848" s="1"/>
       <c r="I848" s="0" t="n">
@@ -23191,13 +23228,13 @@
         <v>843</v>
       </c>
       <c r="B849" s="2" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="C849" s="1" t="s">
         <v>166</v>
       </c>
       <c r="D849" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G849" s="1"/>
       <c r="I849" s="0" t="n">
@@ -23215,13 +23252,13 @@
         <v>844</v>
       </c>
       <c r="B850" s="2" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="C850" s="1" t="s">
         <v>166</v>
       </c>
       <c r="D850" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G850" s="1"/>
       <c r="I850" s="0" t="n">
@@ -23239,13 +23276,13 @@
         <v>845</v>
       </c>
       <c r="B851" s="2" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="C851" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D851" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G851" s="1"/>
       <c r="I851" s="0" t="n">
@@ -23263,13 +23300,13 @@
         <v>846</v>
       </c>
       <c r="B852" s="2" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="C852" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D852" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G852" s="1"/>
       <c r="I852" s="0" t="n">
@@ -23287,13 +23324,13 @@
         <v>847</v>
       </c>
       <c r="B853" s="2" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C853" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D853" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G853" s="1"/>
       <c r="I853" s="0" t="n">
@@ -23311,13 +23348,13 @@
         <v>848</v>
       </c>
       <c r="B854" s="2" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="C854" s="12" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="D854" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G854" s="1"/>
       <c r="I854" s="0" t="n">
@@ -23335,13 +23372,13 @@
         <v>849</v>
       </c>
       <c r="B855" s="2" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="C855" s="12" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="D855" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G855" s="1"/>
       <c r="I855" s="0" t="n">
@@ -23359,13 +23396,13 @@
         <v>850</v>
       </c>
       <c r="B856" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="C856" s="12" t="s">
         <v>941</v>
       </c>
-      <c r="C856" s="12" t="s">
-        <v>939</v>
-      </c>
       <c r="D856" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G856" s="1"/>
       <c r="I856" s="0" t="n">
@@ -23383,13 +23420,13 @@
         <v>851</v>
       </c>
       <c r="B857" s="2" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="C857" s="12" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="D857" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G857" s="1"/>
       <c r="I857" s="0" t="n">
@@ -23407,13 +23444,13 @@
         <v>852</v>
       </c>
       <c r="B858" s="2" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="C858" s="12" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="D858" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G858" s="1"/>
       <c r="I858" s="0" t="n">
@@ -23431,13 +23468,13 @@
         <v>853</v>
       </c>
       <c r="B859" s="2" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="C859" s="12" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="D859" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G859" s="1"/>
       <c r="I859" s="0" t="n">
@@ -23455,13 +23492,13 @@
         <v>854</v>
       </c>
       <c r="B860" s="2" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="C860" s="12" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="D860" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G860" s="1"/>
       <c r="I860" s="0" t="n">
@@ -23479,13 +23516,13 @@
         <v>855</v>
       </c>
       <c r="B861" s="2" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="C861" s="12" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="D861" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G861" s="1"/>
       <c r="I861" s="0" t="n">
@@ -23503,13 +23540,13 @@
         <v>856</v>
       </c>
       <c r="B862" s="2" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="C862" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D862" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G862" s="1"/>
       <c r="I862" s="0" t="n">
@@ -23527,13 +23564,13 @@
         <v>857</v>
       </c>
       <c r="B863" s="2" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="C863" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D863" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G863" s="1"/>
       <c r="I863" s="0" t="n">
@@ -23551,13 +23588,13 @@
         <v>858</v>
       </c>
       <c r="B864" s="2" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C864" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D864" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G864" s="1"/>
       <c r="I864" s="0" t="n">
@@ -23575,13 +23612,13 @@
         <v>859</v>
       </c>
       <c r="B865" s="2" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="C865" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D865" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G865" s="1"/>
       <c r="I865" s="0" t="n">
@@ -23599,13 +23636,13 @@
         <v>860</v>
       </c>
       <c r="B866" s="2" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C866" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D866" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G866" s="1"/>
       <c r="I866" s="0" t="n">
@@ -23623,13 +23660,13 @@
         <v>861</v>
       </c>
       <c r="B867" s="2" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C867" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D867" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G867" s="1"/>
       <c r="I867" s="0" t="n">
@@ -23647,13 +23684,13 @@
         <v>862</v>
       </c>
       <c r="B868" s="2" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="C868" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D868" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G868" s="1"/>
       <c r="I868" s="0" t="n">
@@ -23671,13 +23708,13 @@
         <v>863</v>
       </c>
       <c r="B869" s="2" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D869" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G869" s="1"/>
       <c r="I869" s="0" t="n">
@@ -23695,13 +23732,13 @@
         <v>864</v>
       </c>
       <c r="B870" s="2" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D870" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G870" s="1"/>
       <c r="I870" s="0" t="n">
@@ -23719,13 +23756,13 @@
         <v>865</v>
       </c>
       <c r="B871" s="2" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C871" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D871" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G871" s="1"/>
       <c r="I871" s="0" t="n">
@@ -23743,13 +23780,13 @@
         <v>866</v>
       </c>
       <c r="B872" s="2" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="C872" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D872" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G872" s="1"/>
       <c r="I872" s="0" t="n">
@@ -23767,13 +23804,13 @@
         <v>867</v>
       </c>
       <c r="B873" s="2" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="C873" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D873" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G873" s="1"/>
       <c r="I873" s="0" t="n">
@@ -23791,13 +23828,13 @@
         <v>868</v>
       </c>
       <c r="B874" s="2" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D874" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G874" s="1"/>
       <c r="I874" s="0" t="n">
@@ -23815,13 +23852,13 @@
         <v>869</v>
       </c>
       <c r="B875" s="2" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="C875" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D875" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G875" s="1"/>
       <c r="I875" s="0" t="n">
@@ -23839,13 +23876,13 @@
         <v>870</v>
       </c>
       <c r="B876" s="2" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="C876" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D876" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G876" s="1"/>
       <c r="I876" s="0" t="n">
@@ -23863,13 +23900,13 @@
         <v>871</v>
       </c>
       <c r="B877" s="2" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="C877" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D877" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G877" s="1"/>
       <c r="I877" s="0" t="n">
@@ -23887,13 +23924,13 @@
         <v>872</v>
       </c>
       <c r="B878" s="2" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="C878" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D878" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G878" s="1"/>
       <c r="I878" s="0" t="n">
@@ -23911,13 +23948,13 @@
         <v>873</v>
       </c>
       <c r="B879" s="2" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="C879" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D879" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G879" s="1"/>
       <c r="I879" s="0" t="n">
@@ -23935,13 +23972,13 @@
         <v>874</v>
       </c>
       <c r="B880" s="2" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="C880" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D880" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G880" s="1"/>
       <c r="I880" s="0" t="n">
@@ -23959,13 +23996,13 @@
         <v>875</v>
       </c>
       <c r="B881" s="2" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="C881" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D881" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G881" s="1"/>
       <c r="I881" s="0" t="n">
@@ -23983,13 +24020,13 @@
         <v>876</v>
       </c>
       <c r="B882" s="2" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C882" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D882" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G882" s="1"/>
       <c r="I882" s="0" t="n">
@@ -24007,13 +24044,13 @@
         <v>877</v>
       </c>
       <c r="B883" s="2" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="C883" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D883" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G883" s="1"/>
       <c r="I883" s="0" t="n">
@@ -24031,13 +24068,13 @@
         <v>878</v>
       </c>
       <c r="B884" s="2" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C884" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D884" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G884" s="1"/>
       <c r="I884" s="0" t="n">
@@ -24055,13 +24092,13 @@
         <v>879</v>
       </c>
       <c r="B885" s="2" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="C885" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D885" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G885" s="1"/>
       <c r="I885" s="0" t="n">
@@ -24079,13 +24116,13 @@
         <v>880</v>
       </c>
       <c r="B886" s="2" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="C886" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D886" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G886" s="1"/>
       <c r="I886" s="0" t="n">
@@ -24103,13 +24140,13 @@
         <v>881</v>
       </c>
       <c r="B887" s="2" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="C887" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D887" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G887" s="1"/>
       <c r="I887" s="0" t="n">
@@ -24127,13 +24164,13 @@
         <v>882</v>
       </c>
       <c r="B888" s="2" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C888" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D888" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G888" s="1"/>
       <c r="I888" s="0" t="n">
@@ -24151,13 +24188,13 @@
         <v>883</v>
       </c>
       <c r="B889" s="2" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="C889" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D889" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G889" s="1"/>
       <c r="I889" s="0" t="n">
@@ -24175,13 +24212,13 @@
         <v>884</v>
       </c>
       <c r="B890" s="2" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="C890" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D890" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G890" s="1"/>
       <c r="I890" s="0" t="n">
@@ -24199,13 +24236,13 @@
         <v>885</v>
       </c>
       <c r="B891" s="2" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="C891" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D891" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G891" s="1"/>
       <c r="I891" s="0" t="n">
@@ -24223,13 +24260,13 @@
         <v>886</v>
       </c>
       <c r="B892" s="2" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="C892" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D892" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G892" s="1"/>
       <c r="I892" s="0" t="n">
@@ -24247,13 +24284,13 @@
         <v>887</v>
       </c>
       <c r="B893" s="2" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C893" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D893" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G893" s="1"/>
       <c r="I893" s="0" t="n">
@@ -24271,13 +24308,13 @@
         <v>888</v>
       </c>
       <c r="B894" s="2" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="C894" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D894" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G894" s="1"/>
       <c r="I894" s="0" t="n">
@@ -24295,13 +24332,13 @@
         <v>889</v>
       </c>
       <c r="B895" s="2" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="C895" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D895" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G895" s="1"/>
       <c r="I895" s="0" t="n">
@@ -24319,13 +24356,13 @@
         <v>890</v>
       </c>
       <c r="B896" s="2" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="C896" s="12" t="s">
         <v>173</v>
       </c>
       <c r="D896" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G896" s="1"/>
       <c r="I896" s="0" t="n">
@@ -24343,13 +24380,13 @@
         <v>891</v>
       </c>
       <c r="B897" s="2" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C897" s="12" t="s">
         <v>135</v>
       </c>
       <c r="D897" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G897" s="1"/>
       <c r="I897" s="0" t="n">
@@ -24367,13 +24404,13 @@
         <v>892</v>
       </c>
       <c r="B898" s="2" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="C898" s="12" t="s">
         <v>135</v>
       </c>
       <c r="D898" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G898" s="1"/>
       <c r="I898" s="0" t="n">
@@ -24391,13 +24428,13 @@
         <v>893</v>
       </c>
       <c r="B899" s="2" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="C899" s="12" t="s">
         <v>135</v>
       </c>
       <c r="D899" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G899" s="1"/>
       <c r="I899" s="0" t="n">
@@ -24415,13 +24452,13 @@
         <v>894</v>
       </c>
       <c r="B900" s="2" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="C900" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D900" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G900" s="1"/>
       <c r="I900" s="0" t="n">
@@ -24439,13 +24476,13 @@
         <v>895</v>
       </c>
       <c r="B901" s="2" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C901" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D901" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G901" s="1"/>
       <c r="I901" s="0" t="n">
@@ -24463,13 +24500,13 @@
         <v>896</v>
       </c>
       <c r="B902" s="2" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="C902" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D902" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G902" s="1"/>
       <c r="I902" s="0" t="n">
@@ -24487,13 +24524,13 @@
         <v>897</v>
       </c>
       <c r="B903" s="2" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C903" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D903" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G903" s="1"/>
       <c r="I903" s="0" t="n">
@@ -24511,13 +24548,13 @@
         <v>898</v>
       </c>
       <c r="B904" s="2" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="C904" s="12" t="s">
         <v>164</v>
       </c>
       <c r="D904" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G904" s="1"/>
       <c r="I904" s="0" t="n">
@@ -24535,13 +24572,13 @@
         <v>899</v>
       </c>
       <c r="B905" s="2" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D905" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G905" s="1"/>
       <c r="I905" s="0" t="n">
@@ -24559,13 +24596,13 @@
         <v>900</v>
       </c>
       <c r="B906" s="2" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D906" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G906" s="1"/>
       <c r="I906" s="0" t="n">
@@ -24583,13 +24620,13 @@
         <v>901</v>
       </c>
       <c r="B907" s="2" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="C907" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D907" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G907" s="1"/>
       <c r="I907" s="0" t="n">
@@ -24607,13 +24644,13 @@
         <v>902</v>
       </c>
       <c r="B908" s="2" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D908" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G908" s="1"/>
       <c r="I908" s="0" t="n">
@@ -24631,13 +24668,13 @@
         <v>903</v>
       </c>
       <c r="B909" s="2" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D909" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G909" s="1"/>
       <c r="I909" s="0" t="n">
@@ -24655,13 +24692,13 @@
         <v>904</v>
       </c>
       <c r="B910" s="2" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="C910" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D910" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G910" s="1"/>
       <c r="I910" s="0" t="n">
@@ -24679,13 +24716,13 @@
         <v>905</v>
       </c>
       <c r="B911" s="2" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D911" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G911" s="1"/>
       <c r="I911" s="0" t="n">
@@ -24703,13 +24740,13 @@
         <v>906</v>
       </c>
       <c r="B912" s="2" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D912" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G912" s="1"/>
       <c r="I912" s="0" t="n">
@@ -24727,13 +24764,13 @@
         <v>907</v>
       </c>
       <c r="B913" s="2" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C913" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D913" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G913" s="1"/>
       <c r="I913" s="0" t="n">
@@ -24751,13 +24788,13 @@
         <v>908</v>
       </c>
       <c r="B914" s="2" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D914" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G914" s="1"/>
       <c r="I914" s="0" t="n">
@@ -24775,13 +24812,13 @@
         <v>909</v>
       </c>
       <c r="B915" s="2" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D915" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G915" s="1"/>
       <c r="I915" s="0" t="n">
@@ -24799,13 +24836,13 @@
         <v>910</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="C916" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D916" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G916" s="1"/>
       <c r="I916" s="0" t="n">
@@ -24823,13 +24860,13 @@
         <v>911</v>
       </c>
       <c r="B917" s="2" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D917" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G917" s="1"/>
       <c r="I917" s="0" t="n">
@@ -24847,13 +24884,13 @@
         <v>912</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D918" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G918" s="1"/>
       <c r="I918" s="0" t="n">
@@ -24871,13 +24908,13 @@
         <v>913</v>
       </c>
       <c r="B919" s="2" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="C919" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D919" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G919" s="1"/>
       <c r="I919" s="0" t="n">
@@ -24895,13 +24932,13 @@
         <v>914</v>
       </c>
       <c r="B920" s="2" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D920" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G920" s="1"/>
       <c r="I920" s="0" t="n">
@@ -24919,13 +24956,13 @@
         <v>915</v>
       </c>
       <c r="B921" s="2" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="C921" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D921" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G921" s="1"/>
       <c r="I921" s="0" t="n">
@@ -24943,13 +24980,13 @@
         <v>916</v>
       </c>
       <c r="B922" s="2" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="C922" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D922" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G922" s="1"/>
       <c r="I922" s="0" t="n">
@@ -24967,13 +25004,13 @@
         <v>917</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="C923" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D923" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G923" s="1"/>
       <c r="I923" s="0" t="n">
@@ -24991,13 +25028,13 @@
         <v>918</v>
       </c>
       <c r="B924" s="2" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D924" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G924" s="1"/>
       <c r="I924" s="0" t="n">
@@ -25015,13 +25052,13 @@
         <v>919</v>
       </c>
       <c r="B925" s="2" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D925" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G925" s="1"/>
       <c r="I925" s="0" t="n">
@@ -25039,13 +25076,13 @@
         <v>920</v>
       </c>
       <c r="B926" s="2" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="C926" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D926" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G926" s="1"/>
       <c r="I926" s="0" t="n">
@@ -25063,13 +25100,13 @@
         <v>921</v>
       </c>
       <c r="B927" s="2" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="C927" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D927" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G927" s="1"/>
       <c r="I927" s="0" t="n">
@@ -25087,13 +25124,13 @@
         <v>922</v>
       </c>
       <c r="B928" s="2" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="C928" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D928" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G928" s="1"/>
       <c r="I928" s="0" t="n">
@@ -25111,13 +25148,13 @@
         <v>923</v>
       </c>
       <c r="B929" s="2" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="C929" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D929" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G929" s="1"/>
       <c r="I929" s="0" t="n">
@@ -25135,13 +25172,13 @@
         <v>924</v>
       </c>
       <c r="B930" s="2" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="C930" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D930" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G930" s="1"/>
       <c r="I930" s="0" t="n">
@@ -25159,13 +25196,13 @@
         <v>925</v>
       </c>
       <c r="B931" s="2" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="C931" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D931" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="G931" s="1"/>
       <c r="I931" s="0" t="n">
@@ -27516,35 +27553,35 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27555,7 +27592,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed IFT and added EXIT to database
</commit_message>
<xml_diff>
--- a/newrpl/docs/newRPLCommandDatabase.xlsx
+++ b/newrpl/docs/newRPLCommandDatabase.xlsx
@@ -51,9 +51,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2504" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2507" uniqueCount="1030">
   <si>
     <t xml:space="preserve">Total commands implemented</t>
   </si>
@@ -3133,6 +3134,9 @@
   </si>
   <si>
     <t xml:space="preserve">P*A=L*INV(D)*U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXIT</t>
   </si>
   <si>
     <t xml:space="preserve">Num</t>
@@ -3336,7 +3340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3429,10 +3433,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3521,9 +3521,9 @@
   <dimension ref="A2:J1121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="5" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
+      <selection pane="bottomLeft" activeCell="B934" activeCellId="0" sqref="B934"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3546,14 +3546,14 @@
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="n">
         <f aca="false">COUNTIF(J6:J1001,1)</f>
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="5" t="n">
         <f aca="false">COUNTIF(I6:I1001,1)</f>
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">D2/F2</f>
-        <v>0.539622641509434</v>
+        <v>0.540201005025126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16396,7 +16396,6 @@
       <c r="D555" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E555" s="23"/>
       <c r="F555" s="13"/>
       <c r="G555" s="1" t="s">
         <v>625</v>
@@ -17102,7 +17101,6 @@
       <c r="D584" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E584" s="23"/>
       <c r="F584" s="13"/>
       <c r="G584" s="1" t="s">
         <v>660</v>
@@ -25268,23 +25266,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="933" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="933" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A933" s="1" t="n">
         <f aca="false">A932+1</f>
         <v>927</v>
       </c>
-      <c r="B933" s="1"/>
+      <c r="B933" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C933" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D933" s="1" t="s">
+        <v>870</v>
+      </c>
       <c r="G933" s="1"/>
       <c r="I933" s="0" t="n">
         <f aca="false">IF(ISBLANK(B933),0,IF(D933="N/A",0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J933" s="0" t="n">
         <f aca="false">IF(ISBLANK(D933),0,I933)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="934" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="934" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A934" s="1" t="n">
         <f aca="false">A933+1</f>
         <v>928</v>
@@ -25300,7 +25306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="935" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="935" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A935" s="1" t="n">
         <f aca="false">A934+1</f>
         <v>929</v>
@@ -25316,7 +25322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="936" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="936" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A936" s="1" t="n">
         <f aca="false">A935+1</f>
         <v>930</v>
@@ -25332,7 +25338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="937" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="937" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A937" s="1" t="n">
         <f aca="false">A936+1</f>
         <v>931</v>
@@ -25348,7 +25354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="938" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="938" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A938" s="1" t="n">
         <f aca="false">A937+1</f>
         <v>932</v>
@@ -25364,7 +25370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="939" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="939" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A939" s="1" t="n">
         <f aca="false">A938+1</f>
         <v>933</v>
@@ -25380,7 +25386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="940" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="940" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A940" s="1" t="n">
         <f aca="false">A939+1</f>
         <v>934</v>
@@ -25396,7 +25402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="941" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="941" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A941" s="1" t="n">
         <f aca="false">A940+1</f>
         <v>935</v>
@@ -25412,7 +25418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="942" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="942" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A942" s="1" t="n">
         <f aca="false">A941+1</f>
         <v>936</v>
@@ -25428,7 +25434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="943" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="943" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A943" s="1" t="n">
         <f aca="false">A942+1</f>
         <v>937</v>
@@ -25444,7 +25450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="944" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="944" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A944" s="1" t="n">
         <f aca="false">A943+1</f>
         <v>938</v>
@@ -25460,7 +25466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="945" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="945" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A945" s="1" t="n">
         <f aca="false">A944+1</f>
         <v>939</v>
@@ -25476,7 +25482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="946" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="946" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A946" s="1" t="n">
         <f aca="false">A945+1</f>
         <v>940</v>
@@ -25492,7 +25498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="947" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="947" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A947" s="1" t="n">
         <f aca="false">A946+1</f>
         <v>941</v>
@@ -25508,7 +25514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="948" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="948" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A948" s="1" t="n">
         <f aca="false">A947+1</f>
         <v>942</v>
@@ -25524,7 +25530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="949" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="949" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A949" s="1" t="n">
         <f aca="false">A948+1</f>
         <v>943</v>
@@ -25540,7 +25546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="950" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="950" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A950" s="1" t="n">
         <f aca="false">A949+1</f>
         <v>944</v>
@@ -25556,7 +25562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="951" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="951" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A951" s="1" t="n">
         <f aca="false">A950+1</f>
         <v>945</v>
@@ -25572,7 +25578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="952" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="952" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A952" s="1" t="n">
         <f aca="false">A951+1</f>
         <v>946</v>
@@ -25588,7 +25594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="953" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="953" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A953" s="1" t="n">
         <f aca="false">A952+1</f>
         <v>947</v>
@@ -25604,7 +25610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="954" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="954" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A954" s="1" t="n">
         <f aca="false">A953+1</f>
         <v>948</v>
@@ -25620,7 +25626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="955" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="955" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A955" s="1" t="n">
         <f aca="false">A954+1</f>
         <v>949</v>
@@ -25636,7 +25642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="956" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="956" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A956" s="1" t="n">
         <f aca="false">A955+1</f>
         <v>950</v>
@@ -25652,7 +25658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="957" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="957" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A957" s="1" t="n">
         <f aca="false">A956+1</f>
         <v>951</v>
@@ -25668,7 +25674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="958" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="958" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A958" s="1" t="n">
         <f aca="false">A957+1</f>
         <v>952</v>
@@ -25684,7 +25690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="959" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="959" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A959" s="1" t="n">
         <f aca="false">A958+1</f>
         <v>953</v>
@@ -25700,7 +25706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="960" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="960" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A960" s="1" t="n">
         <f aca="false">A959+1</f>
         <v>954</v>
@@ -25716,7 +25722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="961" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="961" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A961" s="1" t="n">
         <f aca="false">A960+1</f>
         <v>955</v>
@@ -25732,7 +25738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="962" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="962" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A962" s="1" t="n">
         <f aca="false">A961+1</f>
         <v>956</v>
@@ -25748,7 +25754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="963" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="963" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A963" s="1" t="n">
         <f aca="false">A962+1</f>
         <v>957</v>
@@ -25764,7 +25770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="964" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="964" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A964" s="1" t="n">
         <f aca="false">A963+1</f>
         <v>958</v>
@@ -25780,7 +25786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="965" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="965" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A965" s="1" t="n">
         <f aca="false">A964+1</f>
         <v>959</v>
@@ -25796,7 +25802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="966" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="966" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A966" s="1" t="n">
         <f aca="false">A965+1</f>
         <v>960</v>
@@ -25812,7 +25818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="967" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="967" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A967" s="1" t="n">
         <f aca="false">A966+1</f>
         <v>961</v>
@@ -25828,7 +25834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="968" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="968" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A968" s="1" t="n">
         <f aca="false">A967+1</f>
         <v>962</v>
@@ -25844,7 +25850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="969" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="969" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A969" s="1" t="n">
         <f aca="false">A968+1</f>
         <v>963</v>
@@ -25860,7 +25866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="970" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="970" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A970" s="1" t="n">
         <f aca="false">A969+1</f>
         <v>964</v>
@@ -25876,7 +25882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="971" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="971" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A971" s="1" t="n">
         <f aca="false">A970+1</f>
         <v>965</v>
@@ -25892,7 +25898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="972" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="972" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A972" s="1" t="n">
         <f aca="false">A971+1</f>
         <v>966</v>
@@ -25908,7 +25914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="973" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="973" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A973" s="1" t="n">
         <f aca="false">A972+1</f>
         <v>967</v>
@@ -25924,7 +25930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="974" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="974" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A974" s="1" t="n">
         <f aca="false">A973+1</f>
         <v>968</v>
@@ -25940,7 +25946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="975" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="975" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A975" s="1" t="n">
         <f aca="false">A974+1</f>
         <v>969</v>
@@ -25956,7 +25962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="976" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="976" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A976" s="1" t="n">
         <f aca="false">A975+1</f>
         <v>970</v>
@@ -25972,7 +25978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="977" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="977" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A977" s="1" t="n">
         <f aca="false">A976+1</f>
         <v>971</v>
@@ -25988,7 +25994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="978" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="978" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A978" s="1" t="n">
         <f aca="false">A977+1</f>
         <v>972</v>
@@ -26004,7 +26010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="979" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="979" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A979" s="1" t="n">
         <f aca="false">A978+1</f>
         <v>973</v>
@@ -26020,7 +26026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="980" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="980" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A980" s="1" t="n">
         <f aca="false">A979+1</f>
         <v>974</v>
@@ -26036,7 +26042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="981" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="981" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A981" s="1" t="n">
         <f aca="false">A980+1</f>
         <v>975</v>
@@ -26052,7 +26058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="982" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="982" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A982" s="1" t="n">
         <f aca="false">A981+1</f>
         <v>976</v>
@@ -26068,7 +26074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="983" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="983" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A983" s="1" t="n">
         <f aca="false">A982+1</f>
         <v>977</v>
@@ -26084,7 +26090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="984" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="984" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A984" s="1" t="n">
         <f aca="false">A983+1</f>
         <v>978</v>
@@ -26100,7 +26106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="985" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="985" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A985" s="1" t="n">
         <f aca="false">A984+1</f>
         <v>979</v>
@@ -26116,7 +26122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="986" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="986" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A986" s="1" t="n">
         <f aca="false">A985+1</f>
         <v>980</v>
@@ -26132,7 +26138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="987" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="987" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A987" s="1" t="n">
         <f aca="false">A986+1</f>
         <v>981</v>
@@ -26148,7 +26154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="988" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="988" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A988" s="1" t="n">
         <f aca="false">A987+1</f>
         <v>982</v>
@@ -26164,7 +26170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="989" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="989" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A989" s="1" t="n">
         <f aca="false">A988+1</f>
         <v>983</v>
@@ -26180,7 +26186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="990" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="990" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A990" s="1" t="n">
         <f aca="false">A989+1</f>
         <v>984</v>
@@ -26196,7 +26202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="991" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="991" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A991" s="1" t="n">
         <f aca="false">A990+1</f>
         <v>985</v>
@@ -26212,7 +26218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="992" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="992" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A992" s="1" t="n">
         <f aca="false">A991+1</f>
         <v>986</v>
@@ -26228,7 +26234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="993" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="993" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A993" s="1" t="n">
         <f aca="false">A992+1</f>
         <v>987</v>
@@ -26244,7 +26250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="994" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="994" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A994" s="1" t="n">
         <f aca="false">A993+1</f>
         <v>988</v>
@@ -26260,7 +26266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="995" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="995" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A995" s="1" t="n">
         <f aca="false">A994+1</f>
         <v>989</v>
@@ -26276,7 +26282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="996" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="996" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A996" s="1" t="n">
         <f aca="false">A995+1</f>
         <v>990</v>
@@ -26292,7 +26298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="997" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="997" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A997" s="1" t="n">
         <f aca="false">A996+1</f>
         <v>991</v>
@@ -26308,7 +26314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="998" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="998" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A998" s="1" t="n">
         <f aca="false">A997+1</f>
         <v>992</v>
@@ -26324,7 +26330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="999" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="999" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A999" s="1" t="n">
         <f aca="false">A998+1</f>
         <v>993</v>
@@ -27597,46 +27603,46 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>1022</v>
-      </c>
-      <c r="D3" s="24" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>1024</v>
-      </c>
-      <c r="D4" s="24" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>1026</v>
-      </c>
-      <c r="D5" s="24" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added binary data commands. Updated command list.
</commit_message>
<xml_diff>
--- a/newrpl/docs/newRPLCommandDatabase.xlsx
+++ b/newrpl/docs/newRPLCommandDatabase.xlsx
@@ -53,9 +53,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$H$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Commands!$A$5:$G$999</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="1039">
   <si>
     <t xml:space="preserve">Total commands implemented</t>
   </si>
@@ -2291,6 +2292,10 @@
     <t xml:space="preserve">STREAM</t>
   </si>
   <si>
+    <t xml:space="preserve">Stack protection disallows access
+ To old stack data</t>
+  </si>
+  <si>
     <t xml:space="preserve">STURM</t>
   </si>
   <si>
@@ -3144,6 +3149,24 @@
   </si>
   <si>
     <t xml:space="preserve">EXIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBARCHIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBRESTORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBSEND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBRECV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBSTATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USBAUTORECV</t>
   </si>
   <si>
     <t xml:space="preserve">Num</t>
@@ -3528,9 +3551,9 @@
   <dimension ref="A2:J1121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="5" topLeftCell="A753" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D102" activeCellId="0" sqref="D102"/>
+      <selection pane="bottomLeft" activeCell="G554" activeCellId="0" sqref="G554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3553,14 +3576,14 @@
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="n">
         <f aca="false">COUNTIF(J6:J1001,1)</f>
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="5" t="n">
         <f aca="false">COUNTIF(I6:I1001,1)</f>
-        <v>796</v>
+        <v>802</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,7 +3592,7 @@
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">D2/F2</f>
-        <v>0.541457286432161</v>
+        <v>0.544887780548628</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4329,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <f aca="false">A36+1</f>
         <v>31</v>
@@ -4654,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <f aca="false">A50+1</f>
         <v>45</v>
@@ -4776,7 +4799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <f aca="false">A55+1</f>
         <v>50</v>
@@ -4806,7 +4829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <f aca="false">A56+1</f>
         <v>51</v>
@@ -4976,7 +4999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <f aca="false">A63+1</f>
         <v>58</v>
@@ -5000,7 +5023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <f aca="false">A64+1</f>
         <v>59</v>
@@ -5678,7 +5701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
         <f aca="false">A93+1</f>
         <v>88</v>
@@ -5863,7 +5886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
         <f aca="false">A101+1</f>
         <v>96</v>
@@ -5929,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="n">
         <f aca="false">A104+1</f>
         <v>99</v>
@@ -5956,7 +5979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="n">
         <f aca="false">A105+1</f>
         <v>100</v>
@@ -6070,7 +6093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="n">
         <f aca="false">A110+1</f>
         <v>105</v>
@@ -6097,7 +6120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="n">
         <f aca="false">A111+1</f>
         <v>106</v>
@@ -6118,7 +6141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="n">
         <f aca="false">A112+1</f>
         <v>107</v>
@@ -6273,7 +6296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
         <f aca="false">A119+1</f>
         <v>114</v>
@@ -6547,7 +6570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
         <f aca="false">A131+1</f>
         <v>126</v>
@@ -6642,7 +6665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="n">
         <f aca="false">A135+1</f>
         <v>130</v>
@@ -6692,7 +6715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
         <f aca="false">A137+1</f>
         <v>132</v>
@@ -6737,7 +6760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
         <f aca="false">A139+1</f>
         <v>134</v>
@@ -6830,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="n">
         <f aca="false">A143+1</f>
         <v>138</v>
@@ -7013,7 +7036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="n">
         <f aca="false">A151+1</f>
         <v>146</v>
@@ -7040,7 +7063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="n">
         <f aca="false">A152+1</f>
         <v>147</v>
@@ -7324,7 +7347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
         <f aca="false">A164+1</f>
         <v>159</v>
@@ -7396,7 +7419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
         <f aca="false">A167+1</f>
         <v>162</v>
@@ -7423,7 +7446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
         <f aca="false">A168+1</f>
         <v>163</v>
@@ -7821,7 +7844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
         <f aca="false">A185+1</f>
         <v>180</v>
@@ -7845,7 +7868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
         <f aca="false">A186+1</f>
         <v>181</v>
@@ -7871,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
         <f aca="false">A187+1</f>
         <v>182</v>
@@ -8006,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="n">
         <f aca="false">A193+1</f>
         <v>188</v>
@@ -8057,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
         <f aca="false">A195+1</f>
         <v>190</v>
@@ -8084,7 +8107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="n">
         <f aca="false">A196+1</f>
         <v>191</v>
@@ -8494,7 +8517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="n">
         <f aca="false">A214+1</f>
         <v>209</v>
@@ -8881,7 +8904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="n">
         <f aca="false">A231+1</f>
         <v>226</v>
@@ -8905,7 +8928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="n">
         <f aca="false">A232+1</f>
         <v>227</v>
@@ -9816,7 +9839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="n">
         <f aca="false">A272+1</f>
         <v>267</v>
@@ -9840,7 +9863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="n">
         <f aca="false">A273+1</f>
         <v>268</v>
@@ -10455,7 +10478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="n">
         <f aca="false">A299+1</f>
         <v>294</v>
@@ -10656,7 +10679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="n">
         <f aca="false">A308+1</f>
         <v>303</v>
@@ -10864,7 +10887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="n">
         <f aca="false">A317+1</f>
         <v>312</v>
@@ -11122,7 +11145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="n">
         <f aca="false">A328+1</f>
         <v>323</v>
@@ -11242,7 +11265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="n">
         <f aca="false">A333+1</f>
         <v>328</v>
@@ -11465,7 +11488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="n">
         <f aca="false">A342+1</f>
         <v>337</v>
@@ -11786,7 +11809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A357" s="1" t="n">
         <f aca="false">A356+1</f>
         <v>351</v>
@@ -11837,7 +11860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A359" s="1" t="n">
         <f aca="false">A358+1</f>
         <v>353</v>
@@ -11861,7 +11884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A360" s="1" t="n">
         <f aca="false">A359+1</f>
         <v>354</v>
@@ -11888,7 +11911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A361" s="1" t="n">
         <f aca="false">A360+1</f>
         <v>355</v>
@@ -11914,7 +11937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A362" s="1" t="n">
         <f aca="false">A361+1</f>
         <v>356</v>
@@ -11941,7 +11964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A363" s="1" t="n">
         <f aca="false">A362+1</f>
         <v>357</v>
@@ -11965,7 +11988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A364" s="1" t="n">
         <f aca="false">A363+1</f>
         <v>358</v>
@@ -11989,7 +12012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A365" s="1" t="n">
         <f aca="false">A364+1</f>
         <v>359</v>
@@ -12677,7 +12700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="396" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="n">
         <f aca="false">A395+1</f>
         <v>390</v>
@@ -12722,7 +12745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="398" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="n">
         <f aca="false">A397+1</f>
         <v>392</v>
@@ -12746,7 +12769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="399" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="n">
         <f aca="false">A398+1</f>
         <v>393</v>
@@ -12794,7 +12817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="401" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="n">
         <f aca="false">A400+1</f>
         <v>395</v>
@@ -13295,7 +13318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="422" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="n">
         <f aca="false">A421+1</f>
         <v>416</v>
@@ -13936,7 +13959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="449" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A449" s="1" t="n">
         <f aca="false">A448+1</f>
         <v>443</v>
@@ -13960,7 +13983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="450" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A450" s="1" t="n">
         <f aca="false">A449+1</f>
         <v>444</v>
@@ -14125,7 +14148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="457" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A457" s="1" t="n">
         <f aca="false">A456+1</f>
         <v>451</v>
@@ -14662,7 +14685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="481" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A481" s="1" t="n">
         <f aca="false">A480+1</f>
         <v>475</v>
@@ -14770,7 +14793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="486" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A486" s="1" t="n">
         <f aca="false">A485+1</f>
         <v>480</v>
@@ -15009,7 +15032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="496" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="496" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A496" s="1" t="n">
         <f aca="false">A495+1</f>
         <v>490</v>
@@ -15141,7 +15164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="502" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A502" s="1" t="n">
         <f aca="false">A501+1</f>
         <v>496</v>
@@ -15258,7 +15281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="507" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A507" s="1" t="n">
         <f aca="false">A506+1</f>
         <v>501</v>
@@ -15282,7 +15305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="508" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="508" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A508" s="1" t="n">
         <f aca="false">A507+1</f>
         <v>502</v>
@@ -15306,7 +15329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="509" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="509" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A509" s="1" t="n">
         <f aca="false">A508+1</f>
         <v>503</v>
@@ -15641,7 +15664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="524" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="524" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A524" s="1" t="n">
         <f aca="false">A523+1</f>
         <v>518</v>
@@ -15902,7 +15925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="535" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="535" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A535" s="1" t="n">
         <f aca="false">A534+1</f>
         <v>529</v>
@@ -15929,7 +15952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="536" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="536" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A536" s="1" t="n">
         <f aca="false">A535+1</f>
         <v>530</v>
@@ -15998,7 +16021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="539" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="539" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A539" s="1" t="n">
         <f aca="false">A538+1</f>
         <v>533</v>
@@ -16025,7 +16048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="540" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="540" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A540" s="1" t="n">
         <f aca="false">A539+1</f>
         <v>534</v>
@@ -16076,7 +16099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="542" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="542" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A542" s="1" t="n">
         <f aca="false">A541+1</f>
         <v>536</v>
@@ -16245,7 +16268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="549" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="549" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A549" s="1" t="n">
         <f aca="false">A548+1</f>
         <v>543</v>
@@ -16321,7 +16344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="552" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="552" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A552" s="1" t="n">
         <f aca="false">A551+1</f>
         <v>546</v>
@@ -16371,7 +16394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="554" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="554" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A554" s="1" t="n">
         <f aca="false">A553+1</f>
         <v>548</v>
@@ -16395,7 +16418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="555" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="555" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A555" s="1" t="n">
         <f aca="false">A554+1</f>
         <v>549</v>
@@ -16829,7 +16852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="573" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="573" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A573" s="1" t="n">
         <f aca="false">A572+1</f>
         <v>567</v>
@@ -17100,7 +17123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="584" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="584" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A584" s="1" t="n">
         <f aca="false">A583+1</f>
         <v>578</v>
@@ -17130,7 +17153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="585" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="585" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A585" s="1" t="n">
         <f aca="false">A584+1</f>
         <v>579</v>
@@ -17226,7 +17249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="589" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="589" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A589" s="1" t="n">
         <f aca="false">A588+1</f>
         <v>583</v>
@@ -17250,7 +17273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="590" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="590" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A590" s="1" t="n">
         <f aca="false">A589+1</f>
         <v>584</v>
@@ -17325,7 +17348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="593" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="593" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A593" s="1" t="n">
         <f aca="false">A592+1</f>
         <v>587</v>
@@ -17454,7 +17477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="599" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="599" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A599" s="1" t="n">
         <f aca="false">A598+1</f>
         <v>593</v>
@@ -17589,7 +17612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="605" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="605" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A605" s="1" t="n">
         <f aca="false">A604+1</f>
         <v>599</v>
@@ -17659,7 +17682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="608" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="608" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A608" s="1" t="n">
         <f aca="false">A607+1</f>
         <v>602</v>
@@ -18117,7 +18140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="628" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="628" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A628" s="1" t="n">
         <f aca="false">A627+1</f>
         <v>622</v>
@@ -18335,7 +18358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="637" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="637" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A637" s="1" t="n">
         <f aca="false">A636+1</f>
         <v>631</v>
@@ -18385,7 +18408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="639" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="639" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A639" s="1" t="n">
         <f aca="false">A638+1</f>
         <v>633</v>
@@ -18527,7 +18550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="645" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="645" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A645" s="1" t="n">
         <f aca="false">A644+1</f>
         <v>639</v>
@@ -18671,7 +18694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="651" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="651" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A651" s="1" t="n">
         <f aca="false">A650+1</f>
         <v>645</v>
@@ -18848,8 +18871,10 @@
       <c r="D658" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F658" s="15"/>
-      <c r="G658" s="1"/>
+      <c r="F658" s="13"/>
+      <c r="G658" s="19" t="s">
+        <v>740</v>
+      </c>
       <c r="I658" s="0" t="n">
         <f aca="false">IF(ISBLANK(B658),0,IF(D658="N/A",0,1))</f>
         <v>1</v>
@@ -18865,7 +18890,7 @@
         <v>653</v>
       </c>
       <c r="B659" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C659" s="1" t="s">
         <v>27</v>
@@ -18886,7 +18911,7 @@
         <v>654</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C660" s="1" t="s">
         <v>27</v>
@@ -18907,7 +18932,7 @@
         <v>655</v>
       </c>
       <c r="B661" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C661" s="12" t="s">
         <v>127</v>
@@ -18932,7 +18957,7 @@
         <v>656</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C662" s="12" t="s">
         <v>136</v>
@@ -18959,7 +18984,7 @@
         <v>657</v>
       </c>
       <c r="B663" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C663" s="1" t="s">
         <v>27</v>
@@ -18980,7 +19005,7 @@
         <v>658</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C664" s="1" t="s">
         <v>16</v>
@@ -18998,13 +19023,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="665" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="665" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A665" s="1" t="n">
         <f aca="false">A664+1</f>
         <v>659</v>
       </c>
       <c r="B665" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C665" s="1" t="s">
         <v>47</v>
@@ -19022,13 +19047,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="666" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="666" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A666" s="1" t="n">
         <f aca="false">A665+1</f>
         <v>660</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C666" s="1" t="s">
         <v>47</v>
@@ -19052,7 +19077,7 @@
         <v>661</v>
       </c>
       <c r="B667" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C667" s="1" t="s">
         <v>105</v>
@@ -19070,13 +19095,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="668" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="668" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A668" s="1" t="n">
         <f aca="false">A667+1</f>
         <v>662</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C668" s="1" t="s">
         <v>47</v>
@@ -19100,7 +19125,7 @@
         <v>663</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="C669" s="1" t="s">
         <v>82</v>
@@ -19124,7 +19149,7 @@
         <v>664</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C670" s="1" t="s">
         <v>27</v>
@@ -19145,7 +19170,7 @@
         <v>665</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C671" s="1" t="s">
         <v>27</v>
@@ -19166,7 +19191,7 @@
         <v>666</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C672" s="1" t="s">
         <v>27</v>
@@ -19187,7 +19212,7 @@
         <v>667</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C673" s="12" t="s">
         <v>136</v>
@@ -19212,7 +19237,7 @@
         <v>668</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C674" s="1" t="s">
         <v>90</v>
@@ -19236,7 +19261,7 @@
         <v>669</v>
       </c>
       <c r="B675" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C675" s="1" t="s">
         <v>27</v>
@@ -19257,7 +19282,7 @@
         <v>670</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C676" s="1" t="s">
         <v>27</v>
@@ -19278,7 +19303,7 @@
         <v>671</v>
       </c>
       <c r="B677" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C677" s="1" t="s">
         <v>27</v>
@@ -19299,7 +19324,7 @@
         <v>672</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C678" s="1" t="s">
         <v>90</v>
@@ -19323,7 +19348,7 @@
         <v>673</v>
       </c>
       <c r="B679" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C679" s="1" t="s">
         <v>27</v>
@@ -19344,7 +19369,7 @@
         <v>674</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C680" s="1" t="s">
         <v>27</v>
@@ -19365,7 +19390,7 @@
         <v>675</v>
       </c>
       <c r="B681" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C681" s="1" t="s">
         <v>27</v>
@@ -19386,7 +19411,7 @@
         <v>676</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C682" s="1" t="s">
         <v>27</v>
@@ -19407,7 +19432,7 @@
         <v>677</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C683" s="1" t="s">
         <v>219</v>
@@ -19416,7 +19441,7 @@
         <v>43</v>
       </c>
       <c r="G683" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="I683" s="0" t="n">
         <f aca="false">IF(ISBLANK(B683),0,IF(D683="N/A",0,1))</f>
@@ -19433,7 +19458,7 @@
         <v>678</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C684" s="1" t="s">
         <v>53</v>
@@ -19457,7 +19482,7 @@
         <v>679</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C685" s="1" t="s">
         <v>22</v>
@@ -19481,7 +19506,7 @@
         <v>680</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C686" s="1" t="s">
         <v>27</v>
@@ -19502,7 +19527,7 @@
         <v>681</v>
       </c>
       <c r="B687" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C687" s="1" t="s">
         <v>56</v>
@@ -19523,7 +19548,7 @@
         <v>682</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C688" s="12" t="s">
         <v>165</v>
@@ -19547,7 +19572,7 @@
         <v>683</v>
       </c>
       <c r="B689" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C689" s="1" t="s">
         <v>22</v>
@@ -19571,7 +19596,7 @@
         <v>684</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C690" s="1" t="s">
         <v>50</v>
@@ -19595,7 +19620,7 @@
         <v>685</v>
       </c>
       <c r="B691" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C691" s="1" t="s">
         <v>219</v>
@@ -19604,7 +19629,7 @@
         <v>43</v>
       </c>
       <c r="G691" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="I691" s="0" t="n">
         <f aca="false">IF(ISBLANK(B691),0,IF(D691="N/A",0,1))</f>
@@ -19621,7 +19646,7 @@
         <v>686</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C692" s="1" t="s">
         <v>27</v>
@@ -19642,7 +19667,7 @@
         <v>687</v>
       </c>
       <c r="B693" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C693" s="1" t="s">
         <v>56</v>
@@ -19663,7 +19688,7 @@
         <v>688</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C694" s="1" t="s">
         <v>53</v>
@@ -19690,7 +19715,7 @@
         <v>689</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C695" s="1" t="s">
         <v>149</v>
@@ -19705,13 +19730,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="696" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="696" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A696" s="1" t="n">
         <f aca="false">A695+1</f>
         <v>690</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C696" s="1" t="s">
         <v>47</v>
@@ -19732,13 +19757,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="697" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="697" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A697" s="1" t="n">
         <f aca="false">A696+1</f>
         <v>691</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C697" s="1" t="s">
         <v>47</v>
@@ -19748,7 +19773,7 @@
       </c>
       <c r="F697" s="13"/>
       <c r="G697" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H697" s="0" t="n">
         <v>110</v>
@@ -19762,13 +19787,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="698" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="698" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A698" s="1" t="n">
         <f aca="false">A697+1</f>
         <v>692</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C698" s="1" t="s">
         <v>87</v>
@@ -19792,7 +19817,7 @@
         <v>693</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C699" s="1" t="s">
         <v>27</v>
@@ -19813,7 +19838,7 @@
         <v>694</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C700" s="1" t="s">
         <v>27</v>
@@ -19834,7 +19859,7 @@
         <v>695</v>
       </c>
       <c r="B701" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C701" s="1" t="s">
         <v>53</v>
@@ -19858,7 +19883,7 @@
         <v>696</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C702" s="1" t="s">
         <v>27</v>
@@ -19879,7 +19904,7 @@
         <v>697</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C703" s="1" t="s">
         <v>27</v>
@@ -19894,13 +19919,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="704" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="704" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A704" s="1" t="n">
         <f aca="false">A703+1</f>
         <v>698</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C704" s="1" t="s">
         <v>47</v>
@@ -19910,7 +19935,7 @@
       </c>
       <c r="F704" s="13"/>
       <c r="G704" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="H704" s="0" t="n">
         <v>110</v>
@@ -19930,7 +19955,7 @@
         <v>699</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C705" s="1" t="s">
         <v>167</v>
@@ -19954,7 +19979,7 @@
         <v>700</v>
       </c>
       <c r="B706" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C706" s="1" t="s">
         <v>27</v>
@@ -19975,7 +20000,7 @@
         <v>701</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C707" s="1" t="s">
         <v>56</v>
@@ -19996,7 +20021,7 @@
         <v>702</v>
       </c>
       <c r="B708" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C708" s="1" t="s">
         <v>27</v>
@@ -20017,7 +20042,7 @@
         <v>703</v>
       </c>
       <c r="B709" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C709" s="1" t="s">
         <v>50</v>
@@ -20041,7 +20066,7 @@
         <v>704</v>
       </c>
       <c r="B710" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C710" s="1" t="s">
         <v>42</v>
@@ -20065,7 +20090,7 @@
         <v>705</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C711" s="1" t="s">
         <v>53</v>
@@ -20089,7 +20114,7 @@
         <v>706</v>
       </c>
       <c r="B712" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C712" s="1" t="s">
         <v>100</v>
@@ -20110,7 +20135,7 @@
         <v>707</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C713" s="1" t="s">
         <v>100</v>
@@ -20131,7 +20156,7 @@
         <v>708</v>
       </c>
       <c r="B714" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C714" s="1" t="s">
         <v>100</v>
@@ -20152,7 +20177,7 @@
         <v>709</v>
       </c>
       <c r="B715" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C715" s="1" t="s">
         <v>22</v>
@@ -20162,7 +20187,7 @@
       </c>
       <c r="F715" s="14"/>
       <c r="G715" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="I715" s="0" t="n">
         <f aca="false">IF(ISBLANK(B715),0,IF(D715="N/A",0,1))</f>
@@ -20179,7 +20204,7 @@
         <v>710</v>
       </c>
       <c r="B716" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C716" s="12" t="s">
         <v>25</v>
@@ -20204,7 +20229,7 @@
         <v>711</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C717" s="12" t="s">
         <v>25</v>
@@ -20229,7 +20254,7 @@
         <v>712</v>
       </c>
       <c r="B718" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C718" s="1" t="s">
         <v>82</v>
@@ -20253,7 +20278,7 @@
         <v>713</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C719" s="1" t="s">
         <v>42</v>
@@ -20274,7 +20299,7 @@
         <v>714</v>
       </c>
       <c r="B720" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C720" s="1" t="s">
         <v>27</v>
@@ -20295,7 +20320,7 @@
         <v>715</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C721" s="1" t="s">
         <v>42</v>
@@ -20319,7 +20344,7 @@
         <v>716</v>
       </c>
       <c r="B722" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C722" s="1" t="s">
         <v>105</v>
@@ -20343,7 +20368,7 @@
         <v>717</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C723" s="1" t="s">
         <v>105</v>
@@ -20367,7 +20392,7 @@
         <v>718</v>
       </c>
       <c r="B724" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C724" s="12" t="s">
         <v>165</v>
@@ -20391,7 +20416,7 @@
         <v>719</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C725" s="16" t="s">
         <v>184</v>
@@ -20415,7 +20440,7 @@
         <v>720</v>
       </c>
       <c r="B726" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C726" s="1" t="s">
         <v>149</v>
@@ -20436,7 +20461,7 @@
         <v>721</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C727" s="1" t="s">
         <v>149</v>
@@ -20457,7 +20482,7 @@
         <v>722</v>
       </c>
       <c r="B728" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C728" s="1" t="s">
         <v>149</v>
@@ -20478,7 +20503,7 @@
         <v>723</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C729" s="1" t="s">
         <v>149</v>
@@ -20499,7 +20524,7 @@
         <v>724</v>
       </c>
       <c r="B730" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C730" s="12" t="s">
         <v>25</v>
@@ -20518,13 +20543,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="731" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="731" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A731" s="1" t="n">
         <f aca="false">A730+1</f>
         <v>725</v>
       </c>
       <c r="B731" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C731" s="1" t="s">
         <v>47</v>
@@ -20548,13 +20573,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="732" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="732" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A732" s="1" t="n">
         <f aca="false">A731+1</f>
         <v>726</v>
       </c>
       <c r="B732" s="2" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C732" s="1" t="s">
         <v>47</v>
@@ -20578,7 +20603,7 @@
         <v>727</v>
       </c>
       <c r="B733" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C733" s="1" t="s">
         <v>149</v>
@@ -20599,7 +20624,7 @@
         <v>728</v>
       </c>
       <c r="B734" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C734" s="1" t="s">
         <v>42</v>
@@ -20623,7 +20648,7 @@
         <v>729</v>
       </c>
       <c r="B735" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C735" s="1" t="s">
         <v>22</v>
@@ -20644,7 +20669,7 @@
         <v>730</v>
       </c>
       <c r="B736" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C736" s="1" t="s">
         <v>22</v>
@@ -20668,7 +20693,7 @@
         <v>731</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C737" s="1" t="s">
         <v>22</v>
@@ -20689,7 +20714,7 @@
         <v>732</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C738" s="1" t="s">
         <v>22</v>
@@ -20710,7 +20735,7 @@
         <v>733</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C739" s="1" t="s">
         <v>27</v>
@@ -20731,7 +20756,7 @@
         <v>734</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C740" s="1" t="s">
         <v>42</v>
@@ -20741,7 +20766,7 @@
       </c>
       <c r="F740" s="14"/>
       <c r="G740" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="I740" s="0" t="n">
         <f aca="false">IF(ISBLANK(B740),0,IF(D740="N/A",0,1))</f>
@@ -20758,7 +20783,7 @@
         <v>735</v>
       </c>
       <c r="B741" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C741" s="1" t="s">
         <v>53</v>
@@ -20768,7 +20793,7 @@
       </c>
       <c r="F741" s="13"/>
       <c r="G741" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="I741" s="0" t="n">
         <f aca="false">IF(ISBLANK(B741),0,IF(D741="N/A",0,1))</f>
@@ -20785,7 +20810,7 @@
         <v>736</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C742" s="12" t="s">
         <v>165</v>
@@ -20809,7 +20834,7 @@
         <v>737</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C743" s="1" t="s">
         <v>56</v>
@@ -20830,7 +20855,7 @@
         <v>738</v>
       </c>
       <c r="B744" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C744" s="1" t="s">
         <v>82</v>
@@ -20854,7 +20879,7 @@
         <v>739</v>
       </c>
       <c r="B745" s="2" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C745" s="1" t="s">
         <v>149</v>
@@ -20869,13 +20894,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="746" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="746" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A746" s="1" t="n">
         <f aca="false">A745+1</f>
         <v>740</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C746" s="1" t="s">
         <v>87</v>
@@ -20893,13 +20918,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="747" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="747" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A747" s="1" t="n">
         <f aca="false">A746+1</f>
         <v>741</v>
       </c>
       <c r="B747" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C747" s="1" t="s">
         <v>87</v>
@@ -20923,10 +20948,10 @@
         <v>742</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C748" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="G748" s="1"/>
       <c r="I748" s="0" t="n">
@@ -20944,7 +20969,7 @@
         <v>743</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C749" s="16" t="s">
         <v>102</v>
@@ -20968,7 +20993,7 @@
         <v>744</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C750" s="1" t="s">
         <v>167</v>
@@ -20986,13 +21011,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="751" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="751" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A751" s="1" t="n">
         <f aca="false">A750+1</f>
         <v>745</v>
       </c>
       <c r="B751" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C751" s="1" t="s">
         <v>87</v>
@@ -21016,7 +21041,7 @@
         <v>746</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C752" s="1" t="s">
         <v>27</v>
@@ -21031,13 +21056,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="753" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="753" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A753" s="1" t="n">
         <f aca="false">A752+1</f>
         <v>747</v>
       </c>
       <c r="B753" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C753" s="1" t="s">
         <v>87</v>
@@ -21061,7 +21086,7 @@
         <v>748</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C754" s="1" t="s">
         <v>56</v>
@@ -21082,7 +21107,7 @@
         <v>749</v>
       </c>
       <c r="B755" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C755" s="1" t="s">
         <v>12</v>
@@ -21100,13 +21125,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="756" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="756" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A756" s="1" t="n">
         <f aca="false">A755+1</f>
         <v>750</v>
       </c>
       <c r="B756" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C756" s="1" t="s">
         <v>87</v>
@@ -21124,13 +21149,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="757" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="757" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A757" s="1" t="n">
         <f aca="false">A756+1</f>
         <v>751</v>
       </c>
       <c r="B757" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C757" s="1" t="s">
         <v>87</v>
@@ -21154,7 +21179,7 @@
         <v>752</v>
       </c>
       <c r="B758" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C758" s="1" t="s">
         <v>56</v>
@@ -21175,7 +21200,7 @@
         <v>753</v>
       </c>
       <c r="B759" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C759" s="1" t="s">
         <v>56</v>
@@ -21196,7 +21221,7 @@
         <v>754</v>
       </c>
       <c r="B760" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C760" s="1" t="s">
         <v>149</v>
@@ -21217,7 +21242,7 @@
         <v>755</v>
       </c>
       <c r="B761" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C761" s="1" t="s">
         <v>56</v>
@@ -21238,7 +21263,7 @@
         <v>756</v>
       </c>
       <c r="B762" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C762" s="1" t="s">
         <v>56</v>
@@ -21259,7 +21284,7 @@
         <v>757</v>
       </c>
       <c r="B763" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C763" s="1" t="s">
         <v>56</v>
@@ -21280,7 +21305,7 @@
         <v>758</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C764" s="1" t="s">
         <v>56</v>
@@ -21301,7 +21326,7 @@
         <v>759</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C765" s="1" t="s">
         <v>27</v>
@@ -21322,7 +21347,7 @@
         <v>760</v>
       </c>
       <c r="B766" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C766" s="1" t="s">
         <v>219</v>
@@ -21343,7 +21368,7 @@
         <v>761</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C767" s="1" t="s">
         <v>56</v>
@@ -21364,7 +21389,7 @@
         <v>762</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C768" s="1" t="s">
         <v>63</v>
@@ -21389,7 +21414,7 @@
         <v>763</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C769" s="1" t="s">
         <v>80</v>
@@ -21413,7 +21438,7 @@
         <v>764</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C770" s="1" t="s">
         <v>63</v>
@@ -21423,7 +21448,7 @@
       </c>
       <c r="F770" s="14"/>
       <c r="G770" s="1" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="I770" s="0" t="n">
         <f aca="false">IF(ISBLANK(B770),0,IF(D770="N/A",0,1))</f>
@@ -21440,7 +21465,7 @@
         <v>765</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C771" s="1" t="s">
         <v>27</v>
@@ -21461,7 +21486,7 @@
         <v>766</v>
       </c>
       <c r="B772" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C772" s="1" t="s">
         <v>27</v>
@@ -21482,7 +21507,7 @@
         <v>767</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C773" s="1" t="s">
         <v>27</v>
@@ -21503,7 +21528,7 @@
         <v>768</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C774" s="1" t="s">
         <v>149</v>
@@ -21524,7 +21549,7 @@
         <v>769</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C775" s="1" t="s">
         <v>63</v>
@@ -21534,7 +21559,7 @@
       </c>
       <c r="F775" s="14"/>
       <c r="G775" s="1" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="I775" s="0" t="n">
         <f aca="false">IF(ISBLANK(B775),0,IF(D775="N/A",0,1))</f>
@@ -21551,7 +21576,7 @@
         <v>770</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C776" s="1" t="s">
         <v>149</v>
@@ -21572,7 +21597,7 @@
         <v>771</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C777" s="1" t="s">
         <v>149</v>
@@ -21593,7 +21618,7 @@
         <v>772</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C778" s="1" t="s">
         <v>149</v>
@@ -21614,7 +21639,7 @@
         <v>773</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C779" s="1" t="s">
         <v>149</v>
@@ -21635,7 +21660,7 @@
         <v>774</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C780" s="1" t="s">
         <v>149</v>
@@ -21656,7 +21681,7 @@
         <v>775</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C781" s="1" t="s">
         <v>149</v>
@@ -21677,7 +21702,7 @@
         <v>776</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C782" s="1" t="s">
         <v>149</v>
@@ -21698,7 +21723,7 @@
         <v>777</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C783" s="1" t="s">
         <v>149</v>
@@ -21719,13 +21744,13 @@
         <v>778</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C784" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D784" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G784" s="1"/>
       <c r="I784" s="0" t="n">
@@ -21743,13 +21768,13 @@
         <v>779</v>
       </c>
       <c r="B785" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C785" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D785" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G785" s="1"/>
       <c r="I785" s="0" t="n">
@@ -21767,13 +21792,13 @@
         <v>780</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C786" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D786" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G786" s="1"/>
       <c r="I786" s="0" t="n">
@@ -21791,13 +21816,13 @@
         <v>781</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C787" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D787" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G787" s="1"/>
       <c r="I787" s="0" t="n">
@@ -21815,13 +21840,13 @@
         <v>782</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C788" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D788" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G788" s="1"/>
       <c r="I788" s="0" t="n">
@@ -21839,13 +21864,13 @@
         <v>783</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C789" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D789" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G789" s="1"/>
       <c r="I789" s="0" t="n">
@@ -21863,13 +21888,13 @@
         <v>784</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C790" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D790" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G790" s="1"/>
       <c r="I790" s="0" t="n">
@@ -21887,13 +21912,13 @@
         <v>785</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C791" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D791" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G791" s="1"/>
       <c r="I791" s="0" t="n">
@@ -21911,13 +21936,13 @@
         <v>786</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C792" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D792" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G792" s="1"/>
       <c r="I792" s="0" t="n">
@@ -21935,13 +21960,13 @@
         <v>787</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C793" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D793" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G793" s="1"/>
       <c r="I793" s="0" t="n">
@@ -21959,13 +21984,13 @@
         <v>788</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C794" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D794" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G794" s="1"/>
       <c r="I794" s="0" t="n">
@@ -21983,13 +22008,13 @@
         <v>789</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D795" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G795" s="1"/>
       <c r="I795" s="0" t="n">
@@ -22007,13 +22032,13 @@
         <v>790</v>
       </c>
       <c r="B796" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="C796" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="C796" s="1" t="s">
-        <v>884</v>
-      </c>
       <c r="D796" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G796" s="1"/>
       <c r="I796" s="0" t="n">
@@ -22031,13 +22056,13 @@
         <v>791</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D797" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G797" s="1"/>
       <c r="I797" s="0" t="n">
@@ -22055,13 +22080,13 @@
         <v>792</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D798" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G798" s="1"/>
       <c r="I798" s="0" t="n">
@@ -22079,13 +22104,13 @@
         <v>793</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D799" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G799" s="1"/>
       <c r="I799" s="0" t="n">
@@ -22103,13 +22128,13 @@
         <v>794</v>
       </c>
       <c r="B800" s="2" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D800" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G800" s="1"/>
       <c r="I800" s="0" t="n">
@@ -22127,13 +22152,13 @@
         <v>795</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D801" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G801" s="1"/>
       <c r="I801" s="0" t="n">
@@ -22151,13 +22176,13 @@
         <v>796</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C802" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D802" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G802" s="1"/>
       <c r="I802" s="0" t="n">
@@ -22175,13 +22200,13 @@
         <v>797</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C803" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D803" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G803" s="1"/>
       <c r="I803" s="0" t="n">
@@ -22199,13 +22224,13 @@
         <v>798</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C804" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D804" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G804" s="1"/>
       <c r="I804" s="0" t="n">
@@ -22223,13 +22248,13 @@
         <v>799</v>
       </c>
       <c r="B805" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C805" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D805" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G805" s="1"/>
       <c r="I805" s="0" t="n">
@@ -22247,13 +22272,13 @@
         <v>800</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C806" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D806" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G806" s="1"/>
       <c r="I806" s="0" t="n">
@@ -22271,13 +22296,13 @@
         <v>801</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C807" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D807" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G807" s="1"/>
       <c r="I807" s="0" t="n">
@@ -22295,13 +22320,13 @@
         <v>802</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D808" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G808" s="1"/>
       <c r="I808" s="0" t="n">
@@ -22319,13 +22344,13 @@
         <v>803</v>
       </c>
       <c r="B809" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D809" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G809" s="1"/>
       <c r="I809" s="0" t="n">
@@ -22343,13 +22368,13 @@
         <v>804</v>
       </c>
       <c r="B810" s="2" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D810" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G810" s="1"/>
       <c r="I810" s="0" t="n">
@@ -22367,13 +22392,13 @@
         <v>805</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D811" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G811" s="1"/>
       <c r="I811" s="0" t="n">
@@ -22391,13 +22416,13 @@
         <v>806</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D812" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G812" s="1"/>
       <c r="I812" s="0" t="n">
@@ -22415,13 +22440,13 @@
         <v>807</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D813" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G813" s="1"/>
       <c r="I813" s="0" t="n">
@@ -22439,13 +22464,13 @@
         <v>808</v>
       </c>
       <c r="B814" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D814" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G814" s="1"/>
       <c r="I814" s="0" t="n">
@@ -22463,13 +22488,13 @@
         <v>809</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D815" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G815" s="1"/>
       <c r="I815" s="0" t="n">
@@ -22487,13 +22512,13 @@
         <v>810</v>
       </c>
       <c r="B816" s="2" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D816" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G816" s="1"/>
       <c r="I816" s="0" t="n">
@@ -22511,13 +22536,13 @@
         <v>811</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D817" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G817" s="1"/>
       <c r="I817" s="0" t="n">
@@ -22535,13 +22560,13 @@
         <v>812</v>
       </c>
       <c r="B818" s="2" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D818" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G818" s="1"/>
       <c r="I818" s="0" t="n">
@@ -22559,13 +22584,13 @@
         <v>813</v>
       </c>
       <c r="B819" s="2" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D819" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G819" s="1"/>
       <c r="I819" s="0" t="n">
@@ -22583,13 +22608,13 @@
         <v>814</v>
       </c>
       <c r="B820" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D820" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G820" s="1"/>
       <c r="I820" s="0" t="n">
@@ -22607,13 +22632,13 @@
         <v>815</v>
       </c>
       <c r="B821" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D821" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G821" s="1"/>
       <c r="I821" s="0" t="n">
@@ -22631,13 +22656,13 @@
         <v>816</v>
       </c>
       <c r="B822" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D822" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G822" s="1"/>
       <c r="I822" s="0" t="n">
@@ -22655,13 +22680,13 @@
         <v>817</v>
       </c>
       <c r="B823" s="2" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C823" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D823" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G823" s="1"/>
       <c r="I823" s="0" t="n">
@@ -22679,13 +22704,13 @@
         <v>818</v>
       </c>
       <c r="B824" s="2" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C824" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D824" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G824" s="1"/>
       <c r="I824" s="0" t="n">
@@ -22703,13 +22728,13 @@
         <v>819</v>
       </c>
       <c r="B825" s="2" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C825" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D825" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G825" s="1"/>
       <c r="I825" s="0" t="n">
@@ -22727,13 +22752,13 @@
         <v>820</v>
       </c>
       <c r="B826" s="2" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D826" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G826" s="1"/>
       <c r="I826" s="0" t="n">
@@ -22751,13 +22776,13 @@
         <v>821</v>
       </c>
       <c r="B827" s="2" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C827" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D827" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G827" s="1"/>
       <c r="I827" s="0" t="n">
@@ -22775,13 +22800,13 @@
         <v>822</v>
       </c>
       <c r="B828" s="2" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C828" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D828" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G828" s="1"/>
       <c r="I828" s="0" t="n">
@@ -22799,13 +22824,13 @@
         <v>823</v>
       </c>
       <c r="B829" s="2" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C829" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D829" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G829" s="1"/>
       <c r="I829" s="0" t="n">
@@ -22823,13 +22848,13 @@
         <v>824</v>
       </c>
       <c r="B830" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C830" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D830" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G830" s="1"/>
       <c r="I830" s="0" t="n">
@@ -22847,13 +22872,13 @@
         <v>825</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C831" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D831" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G831" s="1"/>
       <c r="I831" s="0" t="n">
@@ -22871,13 +22896,13 @@
         <v>826</v>
       </c>
       <c r="B832" s="2" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C832" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D832" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G832" s="1"/>
       <c r="I832" s="0" t="n">
@@ -22895,13 +22920,13 @@
         <v>827</v>
       </c>
       <c r="B833" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C833" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D833" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G833" s="1"/>
       <c r="I833" s="0" t="n">
@@ -22919,13 +22944,13 @@
         <v>828</v>
       </c>
       <c r="B834" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C834" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D834" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G834" s="1"/>
       <c r="I834" s="0" t="n">
@@ -22943,13 +22968,13 @@
         <v>829</v>
       </c>
       <c r="B835" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C835" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D835" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G835" s="1"/>
       <c r="I835" s="0" t="n">
@@ -22967,13 +22992,13 @@
         <v>830</v>
       </c>
       <c r="B836" s="2" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="C836" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D836" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G836" s="1"/>
       <c r="I836" s="0" t="n">
@@ -22991,13 +23016,13 @@
         <v>831</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C837" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D837" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G837" s="1"/>
       <c r="I837" s="0" t="n">
@@ -23015,13 +23040,13 @@
         <v>832</v>
       </c>
       <c r="B838" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C838" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D838" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G838" s="1"/>
       <c r="I838" s="0" t="n">
@@ -23039,13 +23064,13 @@
         <v>833</v>
       </c>
       <c r="B839" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C839" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D839" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G839" s="1"/>
       <c r="I839" s="0" t="n">
@@ -23063,13 +23088,13 @@
         <v>834</v>
       </c>
       <c r="B840" s="2" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C840" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D840" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G840" s="1"/>
       <c r="I840" s="0" t="n">
@@ -23087,13 +23112,13 @@
         <v>835</v>
       </c>
       <c r="B841" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C841" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D841" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G841" s="1"/>
       <c r="I841" s="0" t="n">
@@ -23111,13 +23136,13 @@
         <v>836</v>
       </c>
       <c r="B842" s="2" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C842" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D842" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G842" s="1"/>
       <c r="I842" s="0" t="n">
@@ -23135,13 +23160,13 @@
         <v>837</v>
       </c>
       <c r="B843" s="2" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C843" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D843" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G843" s="1"/>
       <c r="I843" s="0" t="n">
@@ -23159,13 +23184,13 @@
         <v>838</v>
       </c>
       <c r="B844" s="2" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C844" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D844" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G844" s="1"/>
       <c r="I844" s="0" t="n">
@@ -23183,13 +23208,13 @@
         <v>839</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C845" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D845" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G845" s="1"/>
       <c r="I845" s="0" t="n">
@@ -23207,13 +23232,13 @@
         <v>840</v>
       </c>
       <c r="B846" s="2" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C846" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D846" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G846" s="1"/>
       <c r="I846" s="0" t="n">
@@ -23231,13 +23256,13 @@
         <v>841</v>
       </c>
       <c r="B847" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C847" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D847" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G847" s="1"/>
       <c r="I847" s="0" t="n">
@@ -23255,13 +23280,13 @@
         <v>842</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C848" s="1" t="s">
         <v>90</v>
       </c>
       <c r="D848" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G848" s="1"/>
       <c r="I848" s="0" t="n">
@@ -23279,13 +23304,13 @@
         <v>843</v>
       </c>
       <c r="B849" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C849" s="1" t="s">
         <v>167</v>
       </c>
       <c r="D849" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G849" s="1"/>
       <c r="I849" s="0" t="n">
@@ -23303,13 +23328,13 @@
         <v>844</v>
       </c>
       <c r="B850" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C850" s="1" t="s">
         <v>167</v>
       </c>
       <c r="D850" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G850" s="1"/>
       <c r="I850" s="0" t="n">
@@ -23327,13 +23352,13 @@
         <v>845</v>
       </c>
       <c r="B851" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C851" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D851" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G851" s="1"/>
       <c r="I851" s="0" t="n">
@@ -23351,13 +23376,13 @@
         <v>846</v>
       </c>
       <c r="B852" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C852" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D852" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G852" s="1"/>
       <c r="I852" s="0" t="n">
@@ -23375,13 +23400,13 @@
         <v>847</v>
       </c>
       <c r="B853" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C853" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D853" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G853" s="1"/>
       <c r="I853" s="0" t="n">
@@ -23399,13 +23424,13 @@
         <v>848</v>
       </c>
       <c r="B854" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C854" s="12" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D854" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G854" s="1"/>
       <c r="I854" s="0" t="n">
@@ -23423,13 +23448,13 @@
         <v>849</v>
       </c>
       <c r="B855" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="C855" s="12" t="s">
         <v>945</v>
       </c>
-      <c r="C855" s="12" t="s">
-        <v>944</v>
-      </c>
       <c r="D855" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G855" s="1"/>
       <c r="I855" s="0" t="n">
@@ -23447,13 +23472,13 @@
         <v>850</v>
       </c>
       <c r="B856" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C856" s="12" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D856" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G856" s="1"/>
       <c r="I856" s="0" t="n">
@@ -23471,13 +23496,13 @@
         <v>851</v>
       </c>
       <c r="B857" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C857" s="12" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D857" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G857" s="1"/>
       <c r="I857" s="0" t="n">
@@ -23495,13 +23520,13 @@
         <v>852</v>
       </c>
       <c r="B858" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C858" s="12" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D858" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G858" s="1"/>
       <c r="I858" s="0" t="n">
@@ -23519,13 +23544,13 @@
         <v>853</v>
       </c>
       <c r="B859" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C859" s="12" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D859" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G859" s="1"/>
       <c r="I859" s="0" t="n">
@@ -23543,13 +23568,13 @@
         <v>854</v>
       </c>
       <c r="B860" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C860" s="12" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D860" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G860" s="1"/>
       <c r="I860" s="0" t="n">
@@ -23567,13 +23592,13 @@
         <v>855</v>
       </c>
       <c r="B861" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C861" s="12" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D861" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G861" s="1"/>
       <c r="I861" s="0" t="n">
@@ -23591,13 +23616,13 @@
         <v>856</v>
       </c>
       <c r="B862" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C862" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D862" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G862" s="1"/>
       <c r="I862" s="0" t="n">
@@ -23615,13 +23640,13 @@
         <v>857</v>
       </c>
       <c r="B863" s="2" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="C863" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D863" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G863" s="1"/>
       <c r="I863" s="0" t="n">
@@ -23639,13 +23664,13 @@
         <v>858</v>
       </c>
       <c r="B864" s="2" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="C864" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D864" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G864" s="1"/>
       <c r="I864" s="0" t="n">
@@ -23663,13 +23688,13 @@
         <v>859</v>
       </c>
       <c r="B865" s="2" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C865" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D865" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G865" s="1"/>
       <c r="I865" s="0" t="n">
@@ -23687,13 +23712,13 @@
         <v>860</v>
       </c>
       <c r="B866" s="2" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="C866" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D866" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G866" s="1"/>
       <c r="I866" s="0" t="n">
@@ -23711,13 +23736,13 @@
         <v>861</v>
       </c>
       <c r="B867" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C867" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D867" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G867" s="1"/>
       <c r="I867" s="0" t="n">
@@ -23735,13 +23760,13 @@
         <v>862</v>
       </c>
       <c r="B868" s="2" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C868" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D868" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G868" s="1"/>
       <c r="I868" s="0" t="n">
@@ -23759,13 +23784,13 @@
         <v>863</v>
       </c>
       <c r="B869" s="2" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D869" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G869" s="1"/>
       <c r="I869" s="0" t="n">
@@ -23783,13 +23808,13 @@
         <v>864</v>
       </c>
       <c r="B870" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D870" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G870" s="1"/>
       <c r="I870" s="0" t="n">
@@ -23807,13 +23832,13 @@
         <v>865</v>
       </c>
       <c r="B871" s="2" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C871" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D871" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G871" s="1"/>
       <c r="I871" s="0" t="n">
@@ -23831,13 +23856,13 @@
         <v>866</v>
       </c>
       <c r="B872" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C872" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D872" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G872" s="1"/>
       <c r="I872" s="0" t="n">
@@ -23855,13 +23880,13 @@
         <v>867</v>
       </c>
       <c r="B873" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C873" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D873" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G873" s="1"/>
       <c r="I873" s="0" t="n">
@@ -23879,13 +23904,13 @@
         <v>868</v>
       </c>
       <c r="B874" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D874" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G874" s="1"/>
       <c r="I874" s="0" t="n">
@@ -23903,13 +23928,13 @@
         <v>869</v>
       </c>
       <c r="B875" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C875" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D875" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G875" s="1"/>
       <c r="I875" s="0" t="n">
@@ -23927,13 +23952,13 @@
         <v>870</v>
       </c>
       <c r="B876" s="2" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C876" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D876" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G876" s="1"/>
       <c r="I876" s="0" t="n">
@@ -23951,13 +23976,13 @@
         <v>871</v>
       </c>
       <c r="B877" s="2" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C877" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D877" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G877" s="1"/>
       <c r="I877" s="0" t="n">
@@ -23975,13 +24000,13 @@
         <v>872</v>
       </c>
       <c r="B878" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C878" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D878" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G878" s="1"/>
       <c r="I878" s="0" t="n">
@@ -23999,13 +24024,13 @@
         <v>873</v>
       </c>
       <c r="B879" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C879" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D879" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G879" s="1"/>
       <c r="I879" s="0" t="n">
@@ -24023,13 +24048,13 @@
         <v>874</v>
       </c>
       <c r="B880" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C880" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D880" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G880" s="1"/>
       <c r="I880" s="0" t="n">
@@ -24047,13 +24072,13 @@
         <v>875</v>
       </c>
       <c r="B881" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C881" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D881" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G881" s="1"/>
       <c r="I881" s="0" t="n">
@@ -24071,13 +24096,13 @@
         <v>876</v>
       </c>
       <c r="B882" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="C882" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D882" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G882" s="1"/>
       <c r="I882" s="0" t="n">
@@ -24095,13 +24120,13 @@
         <v>877</v>
       </c>
       <c r="B883" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C883" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D883" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G883" s="1"/>
       <c r="I883" s="0" t="n">
@@ -24119,13 +24144,13 @@
         <v>878</v>
       </c>
       <c r="B884" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C884" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D884" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G884" s="1"/>
       <c r="I884" s="0" t="n">
@@ -24143,13 +24168,13 @@
         <v>879</v>
       </c>
       <c r="B885" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C885" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D885" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G885" s="1"/>
       <c r="I885" s="0" t="n">
@@ -24167,13 +24192,13 @@
         <v>880</v>
       </c>
       <c r="B886" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="C886" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D886" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G886" s="1"/>
       <c r="I886" s="0" t="n">
@@ -24191,13 +24216,13 @@
         <v>881</v>
       </c>
       <c r="B887" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C887" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D887" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G887" s="1"/>
       <c r="I887" s="0" t="n">
@@ -24215,13 +24240,13 @@
         <v>882</v>
       </c>
       <c r="B888" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C888" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D888" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G888" s="1"/>
       <c r="I888" s="0" t="n">
@@ -24239,13 +24264,13 @@
         <v>883</v>
       </c>
       <c r="B889" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C889" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D889" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G889" s="1"/>
       <c r="I889" s="0" t="n">
@@ -24263,13 +24288,13 @@
         <v>884</v>
       </c>
       <c r="B890" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C890" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D890" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G890" s="1"/>
       <c r="I890" s="0" t="n">
@@ -24287,13 +24312,13 @@
         <v>885</v>
       </c>
       <c r="B891" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="C891" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D891" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G891" s="1"/>
       <c r="I891" s="0" t="n">
@@ -24311,13 +24336,13 @@
         <v>886</v>
       </c>
       <c r="B892" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C892" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D892" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G892" s="1"/>
       <c r="I892" s="0" t="n">
@@ -24335,13 +24360,13 @@
         <v>887</v>
       </c>
       <c r="B893" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C893" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D893" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G893" s="1"/>
       <c r="I893" s="0" t="n">
@@ -24359,13 +24384,13 @@
         <v>888</v>
       </c>
       <c r="B894" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C894" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D894" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G894" s="1"/>
       <c r="I894" s="0" t="n">
@@ -24383,13 +24408,13 @@
         <v>889</v>
       </c>
       <c r="B895" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C895" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D895" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G895" s="1"/>
       <c r="I895" s="0" t="n">
@@ -24407,13 +24432,13 @@
         <v>890</v>
       </c>
       <c r="B896" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C896" s="12" t="s">
         <v>174</v>
       </c>
       <c r="D896" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G896" s="1"/>
       <c r="I896" s="0" t="n">
@@ -24431,13 +24456,13 @@
         <v>891</v>
       </c>
       <c r="B897" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C897" s="12" t="s">
         <v>136</v>
       </c>
       <c r="D897" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G897" s="1"/>
       <c r="I897" s="0" t="n">
@@ -24455,13 +24480,13 @@
         <v>892</v>
       </c>
       <c r="B898" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C898" s="12" t="s">
         <v>136</v>
       </c>
       <c r="D898" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G898" s="1"/>
       <c r="I898" s="0" t="n">
@@ -24479,13 +24504,13 @@
         <v>893</v>
       </c>
       <c r="B899" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C899" s="12" t="s">
         <v>136</v>
       </c>
       <c r="D899" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G899" s="1"/>
       <c r="I899" s="0" t="n">
@@ -24503,13 +24528,13 @@
         <v>894</v>
       </c>
       <c r="B900" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C900" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D900" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G900" s="1"/>
       <c r="I900" s="0" t="n">
@@ -24527,13 +24552,13 @@
         <v>895</v>
       </c>
       <c r="B901" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C901" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D901" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G901" s="1"/>
       <c r="I901" s="0" t="n">
@@ -24551,13 +24576,13 @@
         <v>896</v>
       </c>
       <c r="B902" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C902" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D902" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G902" s="1"/>
       <c r="I902" s="0" t="n">
@@ -24575,13 +24600,13 @@
         <v>897</v>
       </c>
       <c r="B903" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="C903" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D903" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G903" s="1"/>
       <c r="I903" s="0" t="n">
@@ -24599,13 +24624,13 @@
         <v>898</v>
       </c>
       <c r="B904" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C904" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D904" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G904" s="1"/>
       <c r="I904" s="0" t="n">
@@ -24623,13 +24648,13 @@
         <v>899</v>
       </c>
       <c r="B905" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D905" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G905" s="1"/>
       <c r="I905" s="0" t="n">
@@ -24647,13 +24672,13 @@
         <v>900</v>
       </c>
       <c r="B906" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D906" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G906" s="1"/>
       <c r="I906" s="0" t="n">
@@ -24671,13 +24696,13 @@
         <v>901</v>
       </c>
       <c r="B907" s="2" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C907" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D907" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G907" s="1"/>
       <c r="I907" s="0" t="n">
@@ -24695,13 +24720,13 @@
         <v>902</v>
       </c>
       <c r="B908" s="2" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D908" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G908" s="1"/>
       <c r="I908" s="0" t="n">
@@ -24719,13 +24744,13 @@
         <v>903</v>
       </c>
       <c r="B909" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D909" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G909" s="1"/>
       <c r="I909" s="0" t="n">
@@ -24743,13 +24768,13 @@
         <v>904</v>
       </c>
       <c r="B910" s="2" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C910" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D910" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G910" s="1"/>
       <c r="I910" s="0" t="n">
@@ -24767,13 +24792,13 @@
         <v>905</v>
       </c>
       <c r="B911" s="2" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D911" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G911" s="1"/>
       <c r="I911" s="0" t="n">
@@ -24791,13 +24816,13 @@
         <v>906</v>
       </c>
       <c r="B912" s="2" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D912" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G912" s="1"/>
       <c r="I912" s="0" t="n">
@@ -24815,13 +24840,13 @@
         <v>907</v>
       </c>
       <c r="B913" s="2" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C913" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D913" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G913" s="1"/>
       <c r="I913" s="0" t="n">
@@ -24839,13 +24864,13 @@
         <v>908</v>
       </c>
       <c r="B914" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D914" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G914" s="1"/>
       <c r="I914" s="0" t="n">
@@ -24863,13 +24888,13 @@
         <v>909</v>
       </c>
       <c r="B915" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D915" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G915" s="1"/>
       <c r="I915" s="0" t="n">
@@ -24887,13 +24912,13 @@
         <v>910</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C916" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D916" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G916" s="1"/>
       <c r="I916" s="0" t="n">
@@ -24911,13 +24936,13 @@
         <v>911</v>
       </c>
       <c r="B917" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D917" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G917" s="1"/>
       <c r="I917" s="0" t="n">
@@ -24935,13 +24960,13 @@
         <v>912</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D918" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G918" s="1"/>
       <c r="I918" s="0" t="n">
@@ -24959,13 +24984,13 @@
         <v>913</v>
       </c>
       <c r="B919" s="2" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C919" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D919" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G919" s="1"/>
       <c r="I919" s="0" t="n">
@@ -24983,13 +25008,13 @@
         <v>914</v>
       </c>
       <c r="B920" s="2" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D920" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G920" s="1"/>
       <c r="I920" s="0" t="n">
@@ -25007,13 +25032,13 @@
         <v>915</v>
       </c>
       <c r="B921" s="2" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C921" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D921" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G921" s="1"/>
       <c r="I921" s="0" t="n">
@@ -25031,13 +25056,13 @@
         <v>916</v>
       </c>
       <c r="B922" s="2" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C922" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D922" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G922" s="1"/>
       <c r="I922" s="0" t="n">
@@ -25055,13 +25080,13 @@
         <v>917</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C923" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D923" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G923" s="1"/>
       <c r="I923" s="0" t="n">
@@ -25079,13 +25104,13 @@
         <v>918</v>
       </c>
       <c r="B924" s="2" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D924" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G924" s="1"/>
       <c r="I924" s="0" t="n">
@@ -25103,13 +25128,13 @@
         <v>919</v>
       </c>
       <c r="B925" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D925" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G925" s="1"/>
       <c r="I925" s="0" t="n">
@@ -25127,13 +25152,13 @@
         <v>920</v>
       </c>
       <c r="B926" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C926" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D926" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G926" s="1"/>
       <c r="I926" s="0" t="n">
@@ -25151,13 +25176,13 @@
         <v>921</v>
       </c>
       <c r="B927" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C927" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D927" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G927" s="1"/>
       <c r="I927" s="0" t="n">
@@ -25175,13 +25200,13 @@
         <v>922</v>
       </c>
       <c r="B928" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C928" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D928" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G928" s="1"/>
       <c r="I928" s="0" t="n">
@@ -25199,13 +25224,13 @@
         <v>923</v>
       </c>
       <c r="B929" s="2" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C929" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D929" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G929" s="1"/>
       <c r="I929" s="0" t="n">
@@ -25223,13 +25248,13 @@
         <v>924</v>
       </c>
       <c r="B930" s="2" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C930" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D930" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G930" s="1"/>
       <c r="I930" s="0" t="n">
@@ -25247,13 +25272,13 @@
         <v>925</v>
       </c>
       <c r="B931" s="2" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C931" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D931" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G931" s="1"/>
       <c r="I931" s="0" t="n">
@@ -25271,16 +25296,16 @@
         <v>926</v>
       </c>
       <c r="B932" s="2" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C932" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D932" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G932" s="1" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I932" s="0" t="n">
         <f aca="false">IF(ISBLANK(B932),0,IF(D932="N/A",0,1))</f>
@@ -25297,13 +25322,13 @@
         <v>927</v>
       </c>
       <c r="B933" s="2" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C933" s="1" t="s">
         <v>165</v>
       </c>
       <c r="D933" s="1" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G933" s="1"/>
       <c r="I933" s="0" t="n">
@@ -25315,100 +25340,148 @@
         <v>1</v>
       </c>
     </row>
-    <row r="934" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="934" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A934" s="1" t="n">
         <f aca="false">A933+1</f>
         <v>928</v>
       </c>
-      <c r="B934" s="1"/>
+      <c r="B934" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C934" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D934" s="1" t="s">
+        <v>873</v>
+      </c>
       <c r="G934" s="1"/>
       <c r="I934" s="0" t="n">
         <f aca="false">IF(ISBLANK(B934),0,IF(D934="N/A",0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J934" s="0" t="n">
         <f aca="false">IF(ISBLANK(D934),0,I934)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="935" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="935" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A935" s="1" t="n">
         <f aca="false">A934+1</f>
         <v>929</v>
       </c>
-      <c r="B935" s="1"/>
+      <c r="B935" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C935" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D935" s="1" t="s">
+        <v>873</v>
+      </c>
       <c r="G935" s="1"/>
       <c r="I935" s="0" t="n">
         <f aca="false">IF(ISBLANK(B935),0,IF(D935="N/A",0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J935" s="0" t="n">
         <f aca="false">IF(ISBLANK(D935),0,I935)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="936" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="936" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A936" s="1" t="n">
         <f aca="false">A935+1</f>
         <v>930</v>
       </c>
-      <c r="B936" s="1"/>
+      <c r="B936" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C936" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D936" s="1" t="s">
+        <v>873</v>
+      </c>
       <c r="G936" s="1"/>
       <c r="I936" s="0" t="n">
         <f aca="false">IF(ISBLANK(B936),0,IF(D936="N/A",0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J936" s="0" t="n">
         <f aca="false">IF(ISBLANK(D936),0,I936)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="937" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="937" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A937" s="1" t="n">
         <f aca="false">A936+1</f>
         <v>931</v>
       </c>
-      <c r="B937" s="1"/>
+      <c r="B937" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C937" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D937" s="1" t="s">
+        <v>873</v>
+      </c>
       <c r="G937" s="1"/>
       <c r="I937" s="0" t="n">
         <f aca="false">IF(ISBLANK(B937),0,IF(D937="N/A",0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J937" s="0" t="n">
         <f aca="false">IF(ISBLANK(D937),0,I937)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="938" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="938" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A938" s="1" t="n">
         <f aca="false">A937+1</f>
         <v>932</v>
       </c>
-      <c r="B938" s="1"/>
+      <c r="B938" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C938" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D938" s="1" t="s">
+        <v>873</v>
+      </c>
       <c r="G938" s="1"/>
       <c r="I938" s="0" t="n">
         <f aca="false">IF(ISBLANK(B938),0,IF(D938="N/A",0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J938" s="0" t="n">
         <f aca="false">IF(ISBLANK(D938),0,I938)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="939" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="939" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A939" s="1" t="n">
         <f aca="false">A938+1</f>
         <v>933</v>
       </c>
-      <c r="B939" s="1"/>
+      <c r="B939" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C939" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D939" s="1" t="s">
+        <v>873</v>
+      </c>
       <c r="G939" s="1"/>
       <c r="I939" s="0" t="n">
         <f aca="false">IF(ISBLANK(B939),0,IF(D939="N/A",0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J939" s="0" t="n">
         <f aca="false">IF(ISBLANK(D939),0,I939)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="940" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27593,9 +27666,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A5:H999">
-    <filterColumn colId="7">
+    <filterColumn colId="2">
       <customFilters and="true">
-        <customFilter operator="equal" val="110"/>
+        <customFilter operator="equal" val="Hardware"/>
       </customFilters>
     </filterColumn>
   </autoFilter>
@@ -27628,35 +27701,35 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>1025</v>
+        <v>1032</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1026</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>1027</v>
+        <v>1034</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1028</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>1029</v>
+        <v>1036</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1030</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27667,7 +27740,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1031</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>